<commit_message>
final update of day
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20016533-B4C1-47AF-8E5C-36A556235CDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386502D5-3E1F-486F-9CDC-0A95563B741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1030,7 +1030,7 @@
                   <c:v>26.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>5.5</c:v>
@@ -1039,7 +1039,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.5</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1304,7 +1304,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -2044,7 +2044,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3722,7 +3722,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>11.5</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4276,7 +4276,7 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4376,6 +4376,9 @@
                 <c:pt idx="9">
                   <c:v>0.5</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4576,7 +4579,7 @@
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8065,7 +8068,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8132,7 +8135,7 @@
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
@@ -8144,11 +8147,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>11.5</v>
+        <v>12.5</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>80.5</v>
+        <v>82</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -8232,8 +8235,8 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="21">
-        <f>AVERAGE(H4:H13)</f>
-        <v>7.15</v>
+        <f>AVERAGE(H4:H14)</f>
+        <v>7.4545454545454541</v>
       </c>
       <c r="B6" s="15">
         <v>1.5</v>
@@ -8498,18 +8501,20 @@
         <v>3</v>
       </c>
       <c r="D14" s="17">
+        <v>3.5</v>
+      </c>
+      <c r="E14" s="17">
+        <v>0</v>
+      </c>
+      <c r="F14" s="17">
+        <v>0</v>
+      </c>
+      <c r="G14" s="17">
         <v>3</v>
-      </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17">
-        <v>0</v>
-      </c>
-      <c r="G14" s="17">
-        <v>2</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10.5</v>
       </c>
       <c r="I14" s="24">
         <v>11</v>
@@ -8602,7 +8607,7 @@
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="19">
         <f>SUM(H11:H17)</f>
-        <v>37</v>
+        <v>38.5</v>
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>

</xml_diff>

<commit_message>
New final update for day
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386502D5-3E1F-486F-9CDC-0A95563B741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38BF918D-B113-40BB-B825-66B62BAC8CC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>Day Count</t>
-  </si>
-  <si>
-    <t>Class</t>
   </si>
   <si>
     <t>Time Spent in Hours for each Class</t>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>Class/Job Search</t>
   </si>
 </sst>
 </file>
@@ -1012,7 +1012,7 @@
                   <c:v>N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Class</c:v>
+                  <c:v>Class/Job Search</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1039,7 +1039,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.5</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1304,7 +1304,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.5</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -2044,7 +2044,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.5</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -3616,7 +3616,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Class</c:v>
+                  <c:v>Class/Job Search</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3722,7 +3722,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>12.5</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4498,7 +4498,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Class</c:v>
+                  <c:v>Class/Job Search</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4579,7 +4579,7 @@
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8094,25 +8094,25 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I1" s="24" t="s">
         <v>1</v>
@@ -8123,7 +8123,7 @@
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
@@ -8147,11 +8147,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>12.5</v>
+        <v>13</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>82</v>
+        <v>82.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -8169,7 +8169,7 @@
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="15">
         <v>1.5</v>
@@ -8202,7 +8202,7 @@
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="15">
         <v>3</v>
@@ -8236,7 +8236,7 @@
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="21">
         <f>AVERAGE(H4:H14)</f>
-        <v>7.4545454545454541</v>
+        <v>7.5</v>
       </c>
       <c r="B6" s="15">
         <v>1.5</v>
@@ -8299,7 +8299,7 @@
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="15">
         <v>1.5</v>
@@ -8362,7 +8362,7 @@
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="15">
         <v>5</v>
@@ -8395,7 +8395,7 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="16">
         <v>7</v>
@@ -8462,7 +8462,7 @@
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" s="17">
         <v>3</v>
@@ -8510,11 +8510,11 @@
         <v>0</v>
       </c>
       <c r="G14" s="17">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" si="1"/>
-        <v>10.5</v>
+        <v>11</v>
       </c>
       <c r="I14" s="24">
         <v>11</v>
@@ -8525,7 +8525,7 @@
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
@@ -8564,7 +8564,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -8585,7 +8585,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
@@ -8607,7 +8607,7 @@
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="19">
         <f>SUM(H11:H17)</f>
-        <v>38.5</v>
+        <v>39</v>
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
@@ -8664,7 +8664,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
@@ -8703,7 +8703,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
@@ -8724,7 +8724,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
@@ -8803,7 +8803,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
@@ -8842,7 +8842,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
@@ -8863,7 +8863,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
@@ -8942,7 +8942,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
@@ -8981,7 +8981,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
@@ -9002,7 +9002,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B39" s="17"/>
       <c r="C39" s="17"/>
@@ -9081,7 +9081,7 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B43" s="17"/>
       <c r="C43" s="17"/>
@@ -9120,7 +9120,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B45" s="17"/>
       <c r="C45" s="17"/>
@@ -9141,7 +9141,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
@@ -9220,7 +9220,7 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B50" s="15"/>
       <c r="C50" s="15"/>
@@ -9259,7 +9259,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B52" s="15"/>
       <c r="C52" s="15"/>
@@ -9280,7 +9280,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B53" s="17"/>
       <c r="C53" s="17"/>
@@ -9359,7 +9359,7 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B57" s="17"/>
       <c r="C57" s="17"/>
@@ -9398,7 +9398,7 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B59" s="17"/>
       <c r="C59" s="17"/>
@@ -9419,7 +9419,7 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B60" s="15"/>
       <c r="C60" s="15"/>
@@ -9498,7 +9498,7 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B64" s="15"/>
       <c r="C64" s="15"/>
@@ -9537,7 +9537,7 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B66" s="15"/>
       <c r="C66" s="15"/>
@@ -9558,7 +9558,7 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B67" s="17"/>
       <c r="C67" s="17"/>
@@ -9673,7 +9673,7 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B73" s="17"/>
       <c r="C73" s="17"/>
@@ -9694,7 +9694,7 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B74" s="15"/>
       <c r="C74" s="15"/>
@@ -9773,7 +9773,7 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B78" s="15"/>
       <c r="C78" s="15"/>
@@ -9812,7 +9812,7 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B80" s="15"/>
       <c r="C80" s="15"/>
@@ -9833,7 +9833,7 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B81" s="17"/>
       <c r="C81" s="17"/>
@@ -9912,7 +9912,7 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B85" s="17"/>
       <c r="C85" s="17"/>
@@ -9951,7 +9951,7 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B87" s="17"/>
       <c r="C87" s="17"/>
@@ -9972,7 +9972,7 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B88" s="15"/>
       <c r="C88" s="15"/>
@@ -10051,7 +10051,7 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B92" s="15"/>
       <c r="C92" s="15"/>
@@ -10090,7 +10090,7 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B94" s="15"/>
       <c r="C94" s="15"/>
@@ -10111,7 +10111,7 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B95" s="17"/>
       <c r="C95" s="17"/>
@@ -10190,7 +10190,7 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B99" s="17"/>
       <c r="C99" s="17"/>
@@ -10211,7 +10211,7 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B100" s="17"/>
       <c r="C100" s="17"/>
@@ -10232,7 +10232,7 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B101" s="17"/>
       <c r="C101" s="17"/>
@@ -10253,7 +10253,7 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B102" s="15"/>
       <c r="C102" s="15"/>
@@ -10369,7 +10369,7 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B108" s="15"/>
       <c r="C108" s="15"/>
@@ -10390,7 +10390,7 @@
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B109" s="17"/>
       <c r="C109" s="17"/>
@@ -10470,7 +10470,7 @@
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B113" s="17"/>
       <c r="C113" s="17"/>
@@ -10509,7 +10509,7 @@
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A115" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B115" s="17"/>
       <c r="C115" s="17"/>
@@ -10530,7 +10530,7 @@
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A116" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B116" s="18"/>
       <c r="C116" s="18"/>
@@ -10591,7 +10591,7 @@
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A119" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B119" s="18"/>
       <c r="C119" s="18"/>

</xml_diff>

<commit_message>
updated - more stats
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6E1B66-03C2-4B94-B7AE-A8681F1D7E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E1F343-E419-4BAE-9BAE-C6D8B2879A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1033,13 +1033,13 @@
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19</c:v>
+                  <c:v>19.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1319,7 +1319,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0</c:v>
@@ -2059,7 +2059,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0</c:v>
@@ -3470,7 +3470,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>14</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3722,7 +3722,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>19</c:v>
+                  <c:v>19.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4434,7 +4434,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4664,6 +4664,9 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8152,7 +8155,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8223,7 +8226,7 @@
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -8231,11 +8234,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>19</v>
+        <v>19.5</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>113</v>
+        <v>114.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -8749,15 +8752,17 @@
         <v>0.5</v>
       </c>
       <c r="E19" s="15">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F19" s="15">
         <v>0</v>
       </c>
-      <c r="G19" s="15"/>
+      <c r="G19" s="15">
+        <v>0.5</v>
+      </c>
       <c r="H19" s="1">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6.5</v>
       </c>
       <c r="I19" s="24">
         <v>16</v>
@@ -8886,7 +8891,7 @@
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="14">
         <f>SUM(H18:H24)</f>
-        <v>15</v>
+        <v>16.5</v>
       </c>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>

</xml_diff>

<commit_message>
updated end notes stat
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E1F343-E419-4BAE-9BAE-C6D8B2879A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B374D739-DA6B-4D5F-97F8-4A45EB15E249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1033,7 +1033,7 @@
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15</c:v>
+                  <c:v>16.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1319,7 +1319,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0</c:v>
@@ -2059,7 +2059,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0</c:v>
@@ -3470,7 +3470,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>16.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4434,7 +4434,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8155,7 +8155,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8226,7 +8226,7 @@
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>15</v>
+        <v>16.5</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -8238,7 +8238,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>114.5</v>
+        <v>116</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -8752,7 +8752,7 @@
         <v>0.5</v>
       </c>
       <c r="E19" s="15">
-        <v>5</v>
+        <v>6.5</v>
       </c>
       <c r="F19" s="15">
         <v>0</v>
@@ -8762,7 +8762,7 @@
       </c>
       <c r="H19" s="1">
         <f t="shared" si="1"/>
-        <v>6.5</v>
+        <v>8</v>
       </c>
       <c r="I19" s="24">
         <v>16</v>
@@ -8891,7 +8891,7 @@
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="14">
         <f>SUM(H18:H24)</f>
-        <v>16.5</v>
+        <v>18</v>
       </c>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>

</xml_diff>

<commit_message>
Mid work progress rep
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BADE2EE-201A-415C-AB26-8EA71210D01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4736E2B-28CF-4EAB-A639-0D52AD99752F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1024,16 +1024,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>34</c:v>
+                  <c:v>34.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33</c:v>
+                  <c:v>33.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>22.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1325,7 +1325,7 @@
                   <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -2065,7 +2065,7 @@
                   <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -3092,7 +3092,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>34</c:v>
+                  <c:v>34.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3218,7 +3218,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>33</c:v>
+                  <c:v>33.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>22</c:v>
+                  <c:v>22.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3470,7 +3470,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>18</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4094,6 +4094,9 @@
                 <c:pt idx="16">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4213,6 +4216,9 @@
                 <c:pt idx="16">
                   <c:v>2</c:v>
                 </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4333,7 +4339,7 @@
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4453,6 +4459,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8185,7 +8194,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8244,19 +8253,19 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>34</v>
+        <v>34.25</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
-        <v>33</v>
+        <v>33.25</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>22</v>
+        <v>22.5</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -8268,7 +8277,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>133.5</v>
+        <v>137.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -8834,12 +8843,18 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
+      <c r="B21" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="C21" s="15">
+        <v>0.25</v>
+      </c>
       <c r="D21" s="15">
-        <v>2.5</v>
-      </c>
-      <c r="E21" s="15"/>
+        <v>3</v>
+      </c>
+      <c r="E21" s="15">
+        <v>3</v>
+      </c>
       <c r="F21" s="15">
         <v>0</v>
       </c>
@@ -8848,7 +8863,7 @@
       </c>
       <c r="H21" s="1">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I21" s="24">
         <v>18</v>
@@ -8941,7 +8956,7 @@
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="14">
         <f>SUM(H18:H24)</f>
-        <v>35.5</v>
+        <v>39.5</v>
       </c>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>

</xml_diff>

<commit_message>
308 work with nate
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09E5E71-B431-4A7E-80B8-CEFF513A0943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60FFFF45-292F-4E5C-9315-C94CC4E780E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1039,7 +1039,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1337,7 +1337,7 @@
                   <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4.5</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0</c:v>
@@ -2077,7 +2077,7 @@
                   <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4.5</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0</c:v>
@@ -3722,7 +3722,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4771,7 +4771,7 @@
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.5</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8259,8 +8259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8339,11 +8339,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -8428,7 +8428,7 @@
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="21">
         <f>AVERAGE(H4:H25)</f>
-        <v>7.5909090909090908</v>
+        <v>7.6363636363636367</v>
       </c>
       <c r="B6" s="15">
         <v>1.5</v>
@@ -9050,11 +9050,11 @@
         <v>0</v>
       </c>
       <c r="G25" s="17">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="H25" s="1">
         <f t="shared" si="1"/>
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="I25" s="24">
         <v>22</v>
@@ -9205,7 +9205,7 @@
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="19">
         <f>SUM(H25:H31)</f>
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>

</xml_diff>

<commit_message>
What is it that you do?
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465400E8-3A0B-4F4D-B103-D4C5F1120FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5324A811-609E-4391-9FC3-BD27634A1926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1030,7 +1030,7 @@
                   <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31.5</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>31</c:v>
@@ -1039,7 +1039,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.5</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1340,10 +1340,10 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9.5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>0</c:v>
@@ -2080,10 +2080,10 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9.5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>0</c:v>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>31.5</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3722,7 +3722,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>32.5</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4386,6 +4386,9 @@
                 <c:pt idx="22">
                   <c:v>1.5</c:v>
                 </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4795,7 +4798,10 @@
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.5</c:v>
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8284,7 +8290,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8351,7 +8357,7 @@
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>31.5</v>
+        <v>32</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
@@ -8363,11 +8369,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>32.5</v>
+        <v>36</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -9112,11 +9118,11 @@
         <v>0</v>
       </c>
       <c r="G26" s="17">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="H26" s="1">
         <f t="shared" si="1"/>
-        <v>9.5</v>
+        <v>10</v>
       </c>
       <c r="I26" s="24">
         <v>23</v>
@@ -9128,13 +9134,17 @@
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
+      <c r="D27" s="17">
+        <v>0.5</v>
+      </c>
       <c r="E27" s="17"/>
       <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
+      <c r="G27" s="17">
+        <v>3</v>
+      </c>
       <c r="H27" s="1">
         <f>SUM(B27:G27)</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="I27" s="24">
         <v>24</v>
@@ -9245,7 +9255,7 @@
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="19">
         <f>SUM(H25:H31)</f>
-        <v>22.5</v>
+        <v>26.5</v>
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>

</xml_diff>

<commit_message>
more work to be done
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C19FA8-22C7-437D-B670-A6E788643A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24793986-5A34-464B-B591-EDF33056B97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1039,7 +1039,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>46</c:v>
+                  <c:v>46.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1346,7 +1346,7 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>8.5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>0</c:v>
@@ -2086,7 +2086,7 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>8.5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>0</c:v>
@@ -3722,7 +3722,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>46</c:v>
+                  <c:v>46.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4831,7 +4831,7 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8319,8 +8319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8399,11 +8399,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>46</v>
+        <v>46.5</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>205</v>
+        <v>205.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -8487,8 +8487,8 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="21">
-        <f>AVERAGE(H4:H27)</f>
-        <v>8.1875</v>
+        <f>AVERAGE(H4:H28)</f>
+        <v>8.2200000000000006</v>
       </c>
       <c r="B6" s="15">
         <v>1.5</v>
@@ -9208,11 +9208,11 @@
         <v>0</v>
       </c>
       <c r="G28" s="17">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="H28" s="1">
         <f>SUM(B28:G28)</f>
-        <v>8.5</v>
+        <v>9</v>
       </c>
       <c r="I28" s="24">
         <v>25</v>
@@ -9305,7 +9305,7 @@
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="19">
         <f>SUM(H25:H31)</f>
-        <v>42.5</v>
+        <v>43</v>
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>

</xml_diff>

<commit_message>
all the team managment
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659B6BA1-BCE6-4123-B278-1894AD82C8F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADADDD09-B908-485F-9C88-F3511EF82EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1030,7 +1030,7 @@
                   <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34.5</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>33.5</c:v>
@@ -1349,7 +1349,7 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4.5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>0</c:v>
@@ -2089,7 +2089,7 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4.5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>0</c:v>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>34.5</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4411,7 +4411,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8337,8 +8337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8405,7 +8405,7 @@
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>34.5</v>
+        <v>36</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
@@ -8421,7 +8421,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>210</v>
+        <v>211.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -9250,7 +9250,7 @@
         <v>1</v>
       </c>
       <c r="D29" s="17">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E29" s="17">
         <v>0.5</v>
@@ -9263,7 +9263,7 @@
       </c>
       <c r="H29" s="1">
         <f>SUM(B29:G29)</f>
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="I29" s="24">
         <v>26</v>
@@ -9335,7 +9335,7 @@
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="19">
         <f>SUM(H25:H31)</f>
-        <v>47.5</v>
+        <v>49</v>
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>

</xml_diff>

<commit_message>
May have committed error
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADADDD09-B908-485F-9C88-F3511EF82EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61291F33-DDBB-45A0-9092-40BE663DE3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1030,7 +1030,7 @@
                   <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>33.5</c:v>
@@ -1349,7 +1349,7 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>0</c:v>
@@ -2089,7 +2089,7 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>0</c:v>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>36</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4411,7 +4411,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.5</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8337,7 +8337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
@@ -8405,7 +8405,7 @@
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
@@ -8421,7 +8421,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>211.5</v>
+        <v>213.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -9250,7 +9250,7 @@
         <v>1</v>
       </c>
       <c r="D29" s="17">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="E29" s="17">
         <v>0.5</v>
@@ -9263,7 +9263,7 @@
       </c>
       <c r="H29" s="1">
         <f>SUM(B29:G29)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I29" s="24">
         <v>26</v>
@@ -9335,7 +9335,7 @@
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="19">
         <f>SUM(H25:H31)</f>
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>

</xml_diff>

<commit_message>
Error encounter longer than exp
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61291F33-DDBB-45A0-9092-40BE663DE3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC403CE-F60E-43BA-87DA-E8DF0C6ED34D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1030,7 +1030,7 @@
                   <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>38</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>33.5</c:v>
@@ -1349,7 +1349,7 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>0</c:v>
@@ -2089,7 +2089,7 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>0</c:v>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>38</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4411,7 +4411,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4.5</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8337,7 +8337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
@@ -8405,7 +8405,7 @@
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
@@ -8421,7 +8421,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>213.5</v>
+        <v>214.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -9250,7 +9250,7 @@
         <v>1</v>
       </c>
       <c r="D29" s="17">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="E29" s="17">
         <v>0.5</v>
@@ -9263,7 +9263,7 @@
       </c>
       <c r="H29" s="1">
         <f>SUM(B29:G29)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I29" s="24">
         <v>26</v>
@@ -9335,7 +9335,7 @@
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="19">
         <f>SUM(H25:H31)</f>
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>

</xml_diff>

<commit_message>
Always more work to do
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A7A5B0-B615-43BB-ADE1-F39B0AD7BBC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16BDC941-B9E9-4DC1-85A8-FA394580A368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1024,13 +1024,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>45.5</c:v>
+                  <c:v>46.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48.5</c:v>
+                  <c:v>49.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40.5</c:v>
+                  <c:v>42.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>34</c:v>
@@ -1039,7 +1039,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1352,7 +1352,7 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>0</c:v>
@@ -2092,7 +2092,7 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>0</c:v>
@@ -3092,7 +3092,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>45.5</c:v>
+                  <c:v>46.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3218,7 +3218,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>48.5</c:v>
+                  <c:v>49.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>40.5</c:v>
+                  <c:v>42.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3722,7 +3722,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4121,6 +4121,9 @@
                 <c:pt idx="25">
                   <c:v>0.5</c:v>
                 </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.75</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4267,6 +4270,9 @@
                 <c:pt idx="25">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.75</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4414,7 +4420,7 @@
                   <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.5</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4711,6 +4717,9 @@
                 <c:pt idx="25">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4858,7 +4867,7 @@
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8346,8 +8355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8406,15 +8415,15 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>45.5</v>
+        <v>46.25</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
-        <v>48.5</v>
+        <v>49.25</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>40.5</v>
+        <v>42.5</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
@@ -8426,11 +8435,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>218.5</v>
+        <v>223</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -9282,21 +9291,27 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
+      <c r="B30" s="17">
+        <v>0.75</v>
+      </c>
+      <c r="C30" s="17">
+        <v>0.75</v>
+      </c>
       <c r="D30" s="17">
-        <v>1.5</v>
+        <v>3.5</v>
       </c>
       <c r="E30" s="17">
         <v>0.5</v>
       </c>
-      <c r="F30" s="17"/>
+      <c r="F30" s="17">
+        <v>0</v>
+      </c>
       <c r="G30" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H30" s="1">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>8.5</v>
       </c>
       <c r="I30" s="24">
         <v>27</v>
@@ -9350,7 +9365,7 @@
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="19">
         <f>SUM(H25:H31)</f>
-        <v>56</v>
+        <v>60.5</v>
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>

</xml_diff>

<commit_message>
Planning with little work
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16BDC941-B9E9-4DC1-85A8-FA394580A368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB4BF03-684C-4B50-925C-6482713C0555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -107,9 +107,6 @@
     <t>End Week Nine</t>
   </si>
   <si>
-    <t>End Week Fifteen</t>
-  </si>
-  <si>
     <t>Week Five Total:</t>
   </si>
   <si>
@@ -191,9 +188,6 @@
     <t>End Week 10</t>
   </si>
   <si>
-    <t>Week 10 Total:</t>
-  </si>
-  <si>
     <t>First Week of Class</t>
   </si>
   <si>
@@ -233,7 +227,13 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>Class/Job Search</t>
+    <t>Class/Job Search/Interview Prep</t>
+  </si>
+  <si>
+    <t>End Week 16</t>
+  </si>
+  <si>
+    <t>Week Sixteen Total:</t>
   </si>
 </sst>
 </file>
@@ -878,8 +878,8 @@
               <c:idx val="3"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="6.2053548571156754E-2"/>
-                  <c:y val="3.8539128799875554E-2"/>
+                  <c:x val="8.8005786236436234E-2"/>
+                  <c:y val="-5.2423985701959268E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -1012,7 +1012,7 @@
                   <c:v>N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Class/Job Search</c:v>
+                  <c:v>Class/Job Search/Interview Prep</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1024,13 +1024,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>46.25</c:v>
+                  <c:v>46.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>49.25</c:v>
+                  <c:v>49.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42.5</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>34</c:v>
@@ -1039,7 +1039,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>51</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1355,7 +1355,7 @@
                   <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>0</c:v>
@@ -2095,7 +2095,7 @@
                   <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>0</c:v>
@@ -3092,7 +3092,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>46.25</c:v>
+                  <c:v>46.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3218,7 +3218,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>49.25</c:v>
+                  <c:v>49.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>42.5</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3616,7 +3616,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Class/Job Search</c:v>
+                  <c:v>Class/Job Search/Interview Prep</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3722,7 +3722,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>51</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4124,6 +4124,9 @@
                 <c:pt idx="26">
                   <c:v>0.75</c:v>
                 </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4273,6 +4276,9 @@
                 <c:pt idx="26">
                   <c:v>0.75</c:v>
                 </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4422,6 +4428,9 @@
                 <c:pt idx="26">
                   <c:v>3.5</c:v>
                 </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4720,6 +4729,9 @@
                 <c:pt idx="26">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4738,7 +4750,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Class/Job Search</c:v>
+                  <c:v>Class/Job Search/Interview Prep</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4868,6 +4880,9 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8355,8 +8370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8382,22 +8397,22 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
@@ -8415,15 +8430,15 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>46.25</v>
+        <v>46.5</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
-        <v>49.25</v>
+        <v>49.5</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>42.5</v>
+        <v>43</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
@@ -8435,11 +8450,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -8490,7 +8505,7 @@
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="15">
         <v>3</v>
@@ -8587,7 +8602,7 @@
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="15">
         <v>1.5</v>
@@ -8750,7 +8765,7 @@
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B13" s="17">
         <v>3</v>
@@ -8813,7 +8828,7 @@
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="17">
         <v>0.5</v>
@@ -9036,7 +9051,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" s="15">
         <v>0.75</v>
@@ -9259,7 +9274,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" s="17">
         <v>0.5</v>
@@ -9324,15 +9339,25 @@
       <c r="A31" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
+      <c r="B31" s="17">
+        <v>0.25</v>
+      </c>
+      <c r="C31" s="17">
+        <v>0.25</v>
+      </c>
+      <c r="D31" s="17">
+        <v>0.5</v>
+      </c>
       <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
+      <c r="F31" s="17">
+        <v>0</v>
+      </c>
+      <c r="G31" s="17">
+        <v>1</v>
+      </c>
       <c r="H31" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I31" s="24">
         <v>28</v>
@@ -9365,7 +9390,7 @@
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="19">
         <f>SUM(H25:H31)</f>
-        <v>60.5</v>
+        <v>62.5</v>
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
@@ -9422,7 +9447,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
@@ -9482,7 +9507,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B39" s="17"/>
       <c r="C39" s="17"/>
@@ -9561,7 +9586,7 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B43" s="17"/>
       <c r="C43" s="17"/>
@@ -9621,7 +9646,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
@@ -9700,7 +9725,7 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B50" s="15"/>
       <c r="C50" s="15"/>
@@ -9760,7 +9785,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B53" s="17"/>
       <c r="C53" s="17"/>
@@ -9839,7 +9864,7 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B57" s="17"/>
       <c r="C57" s="17"/>
@@ -9899,7 +9924,7 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B60" s="15"/>
       <c r="C60" s="15"/>
@@ -9978,7 +10003,7 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B64" s="15"/>
       <c r="C64" s="15"/>
@@ -10038,7 +10063,7 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B67" s="17"/>
       <c r="C67" s="17"/>
@@ -10153,7 +10178,7 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B73" s="17"/>
       <c r="C73" s="17"/>
@@ -10174,7 +10199,7 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="10" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="B74" s="15"/>
       <c r="C74" s="15"/>
@@ -10253,7 +10278,7 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B78" s="15"/>
       <c r="C78" s="15"/>
@@ -10292,7 +10317,7 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B80" s="15"/>
       <c r="C80" s="15"/>
@@ -10313,7 +10338,7 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B81" s="17"/>
       <c r="C81" s="17"/>
@@ -10392,7 +10417,7 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B85" s="17"/>
       <c r="C85" s="17"/>
@@ -10431,7 +10456,7 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B87" s="17"/>
       <c r="C87" s="17"/>
@@ -10452,7 +10477,7 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B88" s="15"/>
       <c r="C88" s="15"/>
@@ -10531,7 +10556,7 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B92" s="15"/>
       <c r="C92" s="15"/>
@@ -10570,7 +10595,7 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B94" s="15"/>
       <c r="C94" s="15"/>
@@ -10591,7 +10616,7 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B95" s="17"/>
       <c r="C95" s="17"/>
@@ -10670,7 +10695,7 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B99" s="17"/>
       <c r="C99" s="17"/>
@@ -10691,7 +10716,7 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B100" s="17"/>
       <c r="C100" s="17"/>
@@ -10712,7 +10737,7 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B101" s="17"/>
       <c r="C101" s="17"/>
@@ -10733,7 +10758,7 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" s="10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B102" s="15"/>
       <c r="C102" s="15"/>
@@ -10811,7 +10836,9 @@
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A106" s="30"/>
+      <c r="A106" t="s">
+        <v>42</v>
+      </c>
       <c r="B106" s="15"/>
       <c r="C106" s="15"/>
       <c r="D106" s="15"/>
@@ -10849,7 +10876,7 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B108" s="15"/>
       <c r="C108" s="15"/>
@@ -10870,7 +10897,7 @@
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109" s="13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B109" s="17"/>
       <c r="C109" s="17"/>
@@ -10949,9 +10976,6 @@
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
-        <v>43</v>
-      </c>
       <c r="B113" s="17"/>
       <c r="C113" s="17"/>
       <c r="D113" s="17"/>
@@ -10989,7 +11013,7 @@
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A115" s="10" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="B115" s="17"/>
       <c r="C115" s="17"/>
@@ -11010,7 +11034,7 @@
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A116" s="10" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="B116" s="18"/>
       <c r="C116" s="18"/>
@@ -11071,7 +11095,7 @@
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A119" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B119" s="18"/>
       <c r="C119" s="18"/>

</xml_diff>

<commit_message>
mount but not booting
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27897C2-7896-42C7-8A8C-F363A0A0210B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8AF64E-348C-410F-B1E5-C2295251985E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1024,7 +1024,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>47</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>53</c:v>
@@ -1039,7 +1039,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>52</c:v>
+                  <c:v>52.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1355,7 +1355,7 @@
                   <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>0</c:v>
@@ -2095,7 +2095,7 @@
                   <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>0</c:v>
@@ -3092,7 +3092,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>47</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3722,7 +3722,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>52</c:v>
+                  <c:v>52.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4125,7 +4125,7 @@
                   <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.75</c:v>
+                  <c:v>1.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4882,7 +4882,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8370,7 +8370,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
@@ -8430,7 +8430,7 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
@@ -8450,11 +8450,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>52</v>
+        <v>52.5</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>229</v>
+        <v>230.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -9340,7 +9340,7 @@
         <v>8</v>
       </c>
       <c r="B31" s="17">
-        <v>0.75</v>
+        <v>1.75</v>
       </c>
       <c r="C31" s="17">
         <v>3.75</v>
@@ -9353,11 +9353,11 @@
         <v>0</v>
       </c>
       <c r="G31" s="17">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="H31" s="1">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7.5</v>
       </c>
       <c r="I31" s="24">
         <v>28</v>
@@ -9390,7 +9390,7 @@
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="19">
         <f>SUM(H25:H31)</f>
-        <v>66.5</v>
+        <v>68</v>
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>

</xml_diff>

<commit_message>
Revisions and brief plan
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76A7C11-B04A-4B8E-9AF8-84426A069E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CA6749-FD2C-4181-A518-83E7751FFAF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1030,7 +1030,7 @@
                   <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>34.5</c:v>
@@ -1355,7 +1355,7 @@
                   <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>10</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>0</c:v>
@@ -2095,7 +2095,7 @@
                   <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>10</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>0</c:v>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>43</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4429,7 +4429,7 @@
                   <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8373,8 +8373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8441,7 +8441,7 @@
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>43</v>
+        <v>43.5</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
@@ -8457,7 +8457,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>233</v>
+        <v>233.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -8542,7 +8542,7 @@
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="21">
         <f>AVERAGE(H4:H31)</f>
-        <v>8.3214285714285712</v>
+        <v>8.3392857142857135</v>
       </c>
       <c r="B6" s="15">
         <v>1.5</v>
@@ -9349,7 +9349,7 @@
         <v>3.75</v>
       </c>
       <c r="D31" s="17">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E31" s="17">
         <v>0.5</v>
@@ -9362,7 +9362,7 @@
       </c>
       <c r="H31" s="1">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="I31" s="24">
         <v>28</v>
@@ -9395,7 +9395,7 @@
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="19">
         <f>SUM(H25:H31)</f>
-        <v>70.5</v>
+        <v>71</v>
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>

</xml_diff>

<commit_message>
late night and early start
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F2B4AD-7096-419D-871D-2A09D0A9C4DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DA9E1A-57C4-4C99-B0ED-B53844274C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1030,16 +1030,16 @@
                   <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43.75</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>52.75</c:v>
+                  <c:v>54.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1358,7 +1358,7 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0</c:v>
+                  <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>0</c:v>
@@ -2098,7 +2098,7 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0</c:v>
+                  <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>0</c:v>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>43.75</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3470,7 +3470,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>34.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3722,7 +3722,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>52.75</c:v>
+                  <c:v>54.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4431,6 +4431,9 @@
                 <c:pt idx="27">
                   <c:v>1.25</c:v>
                 </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4583,6 +4586,9 @@
                 <c:pt idx="27">
                   <c:v>0.5</c:v>
                 </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4733,6 +4739,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -4886,6 +4895,9 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8374,7 +8386,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8441,11 +8453,11 @@
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>43.75</v>
+        <v>44</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>34.5</v>
+        <v>35</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -8453,11 +8465,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>52.75</v>
+        <v>54.25</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>234</v>
+        <v>236.25</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -9377,13 +9389,21 @@
       </c>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
+      <c r="D32" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="E32" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F32" s="15">
+        <v>0</v>
+      </c>
+      <c r="G32" s="15">
+        <v>1.5</v>
+      </c>
       <c r="H32" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.25</v>
       </c>
       <c r="I32" s="24">
         <v>29</v>
@@ -9534,7 +9554,7 @@
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="14">
         <f>SUM(H32:H38)</f>
-        <v>0</v>
+        <v>2.25</v>
       </c>
       <c r="B40" s="17"/>
       <c r="C40" s="17"/>

</xml_diff>

<commit_message>
Motivation has hit all time low
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DA9E1A-57C4-4C99-B0ED-B53844274C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B6E572-F54C-4D4C-BECA-E7BA70E157A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1024,13 +1024,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>50.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>53</c:v>
+                  <c:v>53.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>35</c:v>
@@ -1358,7 +1358,7 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.25</c:v>
+                  <c:v>4.25</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>0</c:v>
@@ -2098,7 +2098,7 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.25</c:v>
+                  <c:v>4.25</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>0</c:v>
@@ -3092,7 +3092,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>50.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3218,7 +3218,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>53</c:v>
+                  <c:v>53.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>44</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4127,6 +4127,9 @@
                 <c:pt idx="27">
                   <c:v>3.75</c:v>
                 </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4279,6 +4282,9 @@
                 <c:pt idx="27">
                   <c:v>3.75</c:v>
                 </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4432,7 +4438,7 @@
                   <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.25</c:v>
+                  <c:v>1.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8385,8 +8391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8445,15 +8451,15 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>50</v>
+        <v>50.5</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
-        <v>53</v>
+        <v>53.5</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
@@ -8469,7 +8475,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>236.25</v>
+        <v>238.25</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -9387,10 +9393,14 @@
       <c r="A32" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
+      <c r="B32" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="C32" s="15">
+        <v>0.5</v>
+      </c>
       <c r="D32" s="15">
-        <v>0.25</v>
+        <v>1.25</v>
       </c>
       <c r="E32" s="15">
         <v>0.5</v>
@@ -9403,7 +9413,7 @@
       </c>
       <c r="H32" s="1">
         <f t="shared" si="1"/>
-        <v>2.25</v>
+        <v>4.25</v>
       </c>
       <c r="I32" s="24">
         <v>29</v>
@@ -9554,7 +9564,7 @@
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="14">
         <f>SUM(H32:H38)</f>
-        <v>2.25</v>
+        <v>4.25</v>
       </c>
       <c r="B40" s="17"/>
       <c r="C40" s="17"/>

</xml_diff>

<commit_message>
Maybe not all time low
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B6E572-F54C-4D4C-BECA-E7BA70E157A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE2A223-724D-462B-892B-53AEB0B1D85A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1030,7 +1030,7 @@
                   <c:v>53.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>35</c:v>
@@ -1358,7 +1358,7 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4.25</c:v>
+                  <c:v>5.25</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>0</c:v>
@@ -2098,7 +2098,7 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4.25</c:v>
+                  <c:v>5.25</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>0</c:v>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>45</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4438,7 +4438,7 @@
                   <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.25</c:v>
+                  <c:v>2.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8391,8 +8391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8459,7 +8459,7 @@
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
@@ -8475,7 +8475,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>238.25</v>
+        <v>239.25</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -9400,7 +9400,7 @@
         <v>0.5</v>
       </c>
       <c r="D32" s="15">
-        <v>1.25</v>
+        <v>2.25</v>
       </c>
       <c r="E32" s="15">
         <v>0.5</v>
@@ -9413,7 +9413,7 @@
       </c>
       <c r="H32" s="1">
         <f t="shared" si="1"/>
-        <v>4.25</v>
+        <v>5.25</v>
       </c>
       <c r="I32" s="24">
         <v>29</v>
@@ -9564,7 +9564,7 @@
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="14">
         <f>SUM(H32:H38)</f>
-        <v>4.25</v>
+        <v>5.25</v>
       </c>
       <c r="B40" s="17"/>
       <c r="C40" s="17"/>

</xml_diff>

<commit_message>
Updated meetings and after work
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC9721E2-FA76-4AEA-8C2E-90DEC9FAF403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A5BC76-3482-4D5E-9516-7E9B11842473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1027,10 +1027,10 @@
                   <c:v>51.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49</c:v>
+                  <c:v>50.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>46.5</c:v>
@@ -1367,7 +1367,7 @@
                   <c:v>7.25</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>8.25</c:v>
+                  <c:v>10.75</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>0</c:v>
@@ -2107,7 +2107,7 @@
                   <c:v>7.25</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>8.25</c:v>
+                  <c:v>10.75</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>0</c:v>
@@ -3218,7 +3218,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>55</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>49</c:v>
+                  <c:v>50.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4301,7 +4301,7 @@
                   <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4465,7 +4465,7 @@
                   <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8445,8 +8445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8509,11 +8509,11 @@
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>49</v>
+        <v>50.5</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
@@ -8529,7 +8529,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>271.25</v>
+        <v>273.75</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -9545,10 +9545,10 @@
         <v>0.25</v>
       </c>
       <c r="C35" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D35" s="15">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="E35" s="15">
         <v>3.5</v>
@@ -9561,7 +9561,7 @@
       </c>
       <c r="H35" s="1">
         <f t="shared" si="1"/>
-        <v>8.25</v>
+        <v>10.75</v>
       </c>
       <c r="I35" s="24">
         <v>32</v>
@@ -9654,7 +9654,7 @@
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="14">
         <f>SUM(H32:H38)</f>
-        <v>37.25</v>
+        <v>39.75</v>
       </c>
       <c r="B40" s="17"/>
       <c r="C40" s="17"/>

</xml_diff>

<commit_message>
stats work through the night
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B6ABE0-3BB3-4CE0-BA43-4940D1C6A3B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1DEE60-8163-4378-8C5F-656EACA6661F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1033,7 +1033,7 @@
                   <c:v>50.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>46.5</c:v>
+                  <c:v>49.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1367,7 +1367,7 @@
                   <c:v>7.25</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>11.25</c:v>
+                  <c:v>14.25</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>0</c:v>
@@ -2107,7 +2107,7 @@
                   <c:v>7.25</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>11.25</c:v>
+                  <c:v>14.25</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>0</c:v>
@@ -3470,7 +3470,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>46.5</c:v>
+                  <c:v>49.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4629,7 +4629,7 @@
                   <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.5</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8445,8 +8445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8517,7 +8517,7 @@
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>46.5</v>
+        <v>49.5</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -8529,7 +8529,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>274.25</v>
+        <v>277.25</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -9551,7 +9551,7 @@
         <v>2</v>
       </c>
       <c r="E35" s="15">
-        <v>3.5</v>
+        <v>6.5</v>
       </c>
       <c r="F35" s="15">
         <v>0</v>
@@ -9561,7 +9561,7 @@
       </c>
       <c r="H35" s="1">
         <f t="shared" si="1"/>
-        <v>11.25</v>
+        <v>14.25</v>
       </c>
       <c r="I35" s="24">
         <v>32</v>
@@ -9654,7 +9654,7 @@
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="14">
         <f>SUM(H32:H38)</f>
-        <v>40.25</v>
+        <v>43.25</v>
       </c>
       <c r="B40" s="17"/>
       <c r="C40" s="17"/>

</xml_diff>

<commit_message>
setup for next hour
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1DEE60-8163-4378-8C5F-656EACA6661F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FDCA430-09B1-45D6-BFAF-59294BE90F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1033,7 +1033,7 @@
                   <c:v>50.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>49.5</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1370,7 +1370,7 @@
                   <c:v>14.25</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>0</c:v>
@@ -2110,7 +2110,7 @@
                   <c:v>14.25</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>0</c:v>
@@ -3470,7 +3470,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>49.5</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4630,6 +4630,9 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8446,7 +8449,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8517,7 +8520,7 @@
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>49.5</v>
+        <v>53</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -8529,7 +8532,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>277.25</v>
+        <v>280.75</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -9577,12 +9580,14 @@
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
       <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
+      <c r="E36" s="15">
+        <v>3.5</v>
+      </c>
       <c r="F36" s="15"/>
       <c r="G36" s="15"/>
       <c r="H36" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="I36" s="24">
         <v>33</v>
@@ -9654,7 +9659,7 @@
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="14">
         <f>SUM(H32:H38)</f>
-        <v>43.25</v>
+        <v>46.75</v>
       </c>
       <c r="B40" s="17"/>
       <c r="C40" s="17"/>

</xml_diff>

<commit_message>
Let the studying begin
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC308FA-DCE2-455C-B813-EFF2C81DA83B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF253B1-14BF-4F2F-AF63-CAF0BB46E09F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1024,7 +1024,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>54.5</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>59</c:v>
@@ -1039,7 +1039,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>72.5</c:v>
+                  <c:v>73.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1379,7 +1379,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>0</c:v>
@@ -2119,7 +2119,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>0</c:v>
@@ -3092,7 +3092,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>54.5</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3722,7 +3722,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>72.5</c:v>
+                  <c:v>73.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4148,6 +4148,9 @@
                 <c:pt idx="34">
                   <c:v>2.5</c:v>
                 </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4840,6 +4843,9 @@
                 <c:pt idx="34">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="35">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5012,6 +5018,9 @@
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8500,7 +8509,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8559,7 +8568,7 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>54.5</v>
+        <v>56</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
@@ -8579,11 +8588,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>72.5</v>
+        <v>73.5</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>297.5</v>
+        <v>300</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -9724,15 +9733,21 @@
       <c r="A39" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B39" s="17"/>
+      <c r="B39" s="17">
+        <v>1.5</v>
+      </c>
       <c r="C39" s="17"/>
       <c r="D39" s="17"/>
       <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
+      <c r="F39" s="17">
+        <v>0</v>
+      </c>
+      <c r="G39" s="17">
+        <v>1</v>
+      </c>
       <c r="H39" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="I39" s="24">
         <v>36</v>
@@ -9883,7 +9898,7 @@
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="19">
         <f>SUM(H39:H45)</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>

</xml_diff>

<commit_message>
meeting and study remain
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE720BE-B866-40A6-B161-FDC864B46414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3A21C5-2218-47D4-B544-433EB34BB365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1027,7 +1027,7 @@
                   <c:v>58.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59</c:v>
+                  <c:v>59.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>56</c:v>
@@ -1379,7 +1379,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>7.5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>0</c:v>
@@ -2119,7 +2119,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>7.5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>0</c:v>
@@ -3218,7 +3218,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>59</c:v>
+                  <c:v>59.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4323,6 +4323,9 @@
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8514,8 +8517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8578,7 +8581,7 @@
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
-        <v>59</v>
+        <v>59.5</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
@@ -8598,7 +8601,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>305</v>
+        <v>305.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -9742,7 +9745,9 @@
       <c r="B39" s="17">
         <v>4</v>
       </c>
-      <c r="C39" s="17"/>
+      <c r="C39" s="17">
+        <v>0.5</v>
+      </c>
       <c r="D39" s="17">
         <v>1</v>
       </c>
@@ -9757,7 +9762,7 @@
       </c>
       <c r="H39" s="1">
         <f t="shared" si="1"/>
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="I39" s="24">
         <v>36</v>
@@ -9908,7 +9913,7 @@
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="19">
         <f>SUM(H39:H45)</f>
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>

</xml_diff>

<commit_message>
meeting and proj setup
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3A21C5-2218-47D4-B544-433EB34BB365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E4F4B9-5DAB-4F12-ADA6-1D5B3199D592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1030,7 +1030,7 @@
                   <c:v>59.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>56</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>58</c:v>
@@ -1379,7 +1379,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>0</c:v>
@@ -2119,7 +2119,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>0</c:v>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>56</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4501,7 +4501,7 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8517,8 +8517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8585,7 +8585,7 @@
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
@@ -8601,7 +8601,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>305.5</v>
+        <v>307.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -9749,7 +9749,7 @@
         <v>0.5</v>
       </c>
       <c r="D39" s="17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E39" s="17">
         <v>1.5</v>
@@ -9762,7 +9762,7 @@
       </c>
       <c r="H39" s="1">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I39" s="24">
         <v>36</v>
@@ -9913,7 +9913,7 @@
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="19">
         <f>SUM(H39:H45)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>

</xml_diff>

<commit_message>
Time to rule your mind
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90218D5-970E-41FE-A55B-A8457661EC25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F92B0189-9CE2-4F2C-A8BE-690DC675CF61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1027,13 +1027,13 @@
                   <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60.5</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>63</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1382,7 +1382,7 @@
                   <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>8.5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>0</c:v>
@@ -2122,7 +2122,7 @@
                   <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>8.5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>0</c:v>
@@ -3218,7 +3218,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>60.5</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3470,7 +3470,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>63</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4331,7 +4331,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4689,7 +4689,7 @@
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8536,7 +8536,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8599,7 +8599,7 @@
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
-        <v>60.5</v>
+        <v>61</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
@@ -8607,7 +8607,7 @@
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -8619,7 +8619,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>317.5</v>
+        <v>319</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -8704,7 +8704,7 @@
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="21">
         <f>AVERAGE(H4:H40)</f>
-        <v>8.5810810810810807</v>
+        <v>8.621621621621621</v>
       </c>
       <c r="B6" s="15">
         <v>1.5</v>
@@ -9798,13 +9798,13 @@
         <v>0.5</v>
       </c>
       <c r="C40" s="17">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D40" s="17">
         <v>1</v>
       </c>
       <c r="E40" s="17">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F40" s="17">
         <v>0</v>
@@ -9814,7 +9814,7 @@
       </c>
       <c r="H40" s="1">
         <f t="shared" si="1"/>
-        <v>8.5</v>
+        <v>10</v>
       </c>
       <c r="I40" s="24">
         <v>37</v>
@@ -9943,7 +9943,7 @@
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="19">
         <f>SUM(H39:H45)</f>
-        <v>20</v>
+        <v>21.5</v>
       </c>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>

</xml_diff>

<commit_message>
Interview prep arc continues
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17443C13-1C84-46ED-814C-400E6D6F0BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D17AB7-1312-4DC6-84D9-1711C1217BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1039,7 +1039,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>76</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1385,7 +1385,7 @@
                   <c:v>10.25</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4.25</c:v>
+                  <c:v>8.25</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>0</c:v>
@@ -2125,7 +2125,7 @@
                   <c:v>10.25</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4.25</c:v>
+                  <c:v>8.25</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>0</c:v>
@@ -3722,7 +3722,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>76</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4336,6 +4336,9 @@
                 <c:pt idx="36">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5062,7 +5065,7 @@
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8551,7 +8554,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8630,11 +8633,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>323.5</v>
+        <v>327.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -9842,7 +9845,9 @@
       <c r="B41" s="17">
         <v>1.75</v>
       </c>
-      <c r="C41" s="17"/>
+      <c r="C41" s="17">
+        <v>0</v>
+      </c>
       <c r="D41" s="17">
         <v>1</v>
       </c>
@@ -9853,11 +9858,11 @@
         <v>0</v>
       </c>
       <c r="G41" s="17">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H41" s="1">
         <f t="shared" si="1"/>
-        <v>4.25</v>
+        <v>8.25</v>
       </c>
       <c r="I41" s="24">
         <v>38</v>
@@ -9968,7 +9973,7 @@
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="19">
         <f>SUM(H39:H45)</f>
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>

</xml_diff>

<commit_message>
Interview prep arc pt 4
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D17AB7-1312-4DC6-84D9-1711C1217BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0388A83-2F0E-498B-978B-B49D1CD0FDF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1039,7 +1039,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>80</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1385,7 +1385,7 @@
                   <c:v>10.25</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>8.25</c:v>
+                  <c:v>10.25</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>0</c:v>
@@ -2125,7 +2125,7 @@
                   <c:v>10.25</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>8.25</c:v>
+                  <c:v>10.25</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>0</c:v>
@@ -3722,7 +3722,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>80</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5065,7 +5065,7 @@
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8633,11 +8633,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>327.5</v>
+        <v>329.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -9858,11 +9858,11 @@
         <v>0</v>
       </c>
       <c r="G41" s="17">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H41" s="1">
         <f t="shared" si="1"/>
-        <v>8.25</v>
+        <v>10.25</v>
       </c>
       <c r="I41" s="24">
         <v>38</v>
@@ -9973,7 +9973,7 @@
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="19">
         <f>SUM(H39:H45)</f>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>

</xml_diff>

<commit_message>
Interview training arc continues
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0388A83-2F0E-498B-978B-B49D1CD0FDF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F03261-2CA9-459A-986D-FAEB319806DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1039,7 +1039,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>82</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1385,7 +1385,7 @@
                   <c:v>10.25</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>10.25</c:v>
+                  <c:v>11.25</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>0</c:v>
@@ -2125,7 +2125,7 @@
                   <c:v>10.25</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>10.25</c:v>
+                  <c:v>11.25</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>0</c:v>
@@ -3722,7 +3722,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>82</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5065,7 +5065,7 @@
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8633,11 +8633,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>329.5</v>
+        <v>330.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -9858,11 +9858,11 @@
         <v>0</v>
       </c>
       <c r="G41" s="17">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H41" s="1">
         <f t="shared" si="1"/>
-        <v>10.25</v>
+        <v>11.25</v>
       </c>
       <c r="I41" s="24">
         <v>38</v>
@@ -9973,7 +9973,7 @@
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="19">
         <f>SUM(H39:H45)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>

</xml_diff>

<commit_message>
Training arc never ends
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F03261-2CA9-459A-986D-FAEB319806DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A16C83F9-2847-44EB-8B47-742E9E6425CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1039,7 +1039,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>83</c:v>
+                  <c:v>83.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1385,7 +1385,7 @@
                   <c:v>10.25</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>11.25</c:v>
+                  <c:v>11.75</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>0</c:v>
@@ -2125,7 +2125,7 @@
                   <c:v>10.25</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>11.25</c:v>
+                  <c:v>11.75</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>0</c:v>
@@ -3722,7 +3722,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>83</c:v>
+                  <c:v>83.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5065,7 +5065,7 @@
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>8</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8633,11 +8633,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>83</v>
+        <v>83.5</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>330.5</v>
+        <v>331</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -9858,11 +9858,11 @@
         <v>0</v>
       </c>
       <c r="G41" s="17">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="H41" s="1">
         <f t="shared" si="1"/>
-        <v>11.25</v>
+        <v>11.75</v>
       </c>
       <c r="I41" s="24">
         <v>38</v>
@@ -9973,7 +9973,7 @@
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="19">
         <f>SUM(H39:H45)</f>
-        <v>33</v>
+        <v>33.5</v>
       </c>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>

</xml_diff>

<commit_message>
training arc continues in morn
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414AF40D-BAC8-4166-B6C1-23D28148FEB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946BB1D8-DA19-4F2A-9C5A-AB7F1C1DD76A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1039,7 +1039,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>84</c:v>
+                  <c:v>86.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1388,7 +1388,7 @@
                   <c:v>12.25</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>0</c:v>
@@ -2128,7 +2128,7 @@
                   <c:v>12.25</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>0</c:v>
@@ -3722,7 +3722,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>84</c:v>
+                  <c:v>86.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4885,6 +4885,9 @@
                 <c:pt idx="37">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="38">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5066,6 +5069,9 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8553,8 +8559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8633,11 +8639,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>84</v>
+        <v>86.5</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>331.5</v>
+        <v>334</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -9876,11 +9882,15 @@
       <c r="C42" s="17"/>
       <c r="D42" s="17"/>
       <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
+      <c r="F42" s="17">
+        <v>0</v>
+      </c>
+      <c r="G42" s="17">
+        <v>2.5</v>
+      </c>
       <c r="H42" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="I42" s="24">
         <v>39</v>
@@ -9973,7 +9983,7 @@
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="19">
         <f>SUM(H39:H45)</f>
-        <v>34</v>
+        <v>36.5</v>
       </c>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>

</xml_diff>

<commit_message>
hw and study arc
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87B35E3-3F1E-4F46-9166-8D231DFB345C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA29F8CB-22A9-4C15-8F81-448A19B87428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1030,7 +1030,7 @@
                   <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>61</c:v>
+                  <c:v>61.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>64.5</c:v>
@@ -1388,7 +1388,7 @@
                   <c:v>12.25</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>9</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>0</c:v>
@@ -2128,7 +2128,7 @@
                   <c:v>12.25</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>9</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>0</c:v>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>61</c:v>
+                  <c:v>61.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4342,6 +4342,9 @@
                 <c:pt idx="37">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="38">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4523,6 +4526,9 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8562,8 +8568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8630,7 +8636,7 @@
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>61</v>
+        <v>61.5</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
@@ -8646,7 +8652,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>340.5</v>
+        <v>341</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -8730,8 +8736,8 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="21">
-        <f>AVERAGE(H4:H40)</f>
-        <v>8.628378378378379</v>
+        <f>AVERAGE(H4:H42)</f>
+        <v>8.7435897435897427</v>
       </c>
       <c r="B6" s="15">
         <v>1.5</v>
@@ -9884,8 +9890,12 @@
       <c r="B42" s="17">
         <v>0.5</v>
       </c>
-      <c r="C42" s="17"/>
-      <c r="D42" s="17"/>
+      <c r="C42" s="17">
+        <v>0</v>
+      </c>
+      <c r="D42" s="17">
+        <v>0.5</v>
+      </c>
       <c r="E42" s="17"/>
       <c r="F42" s="17">
         <v>0</v>
@@ -9895,7 +9905,7 @@
       </c>
       <c r="H42" s="1">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="I42" s="24">
         <v>39</v>
@@ -9988,7 +9998,7 @@
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="19">
         <f>SUM(H39:H45)</f>
-        <v>43</v>
+        <v>43.5</v>
       </c>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>

</xml_diff>

<commit_message>
Bernoulli be my guide
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D6EDF8-3FCE-43B8-A61A-BFDFFF9FAAB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C0E3C2-B37C-4C7E-B8A9-73B6F0287952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1033,7 +1033,7 @@
                   <c:v>61.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>68</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1388,7 +1388,7 @@
                   <c:v>12.25</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>13</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>0</c:v>
@@ -2128,7 +2128,7 @@
                   <c:v>12.25</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>13</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>0</c:v>
@@ -3470,7 +3470,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>68</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4713,7 +4713,7 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>3.5</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8572,7 +8572,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8643,7 +8643,7 @@
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -8655,7 +8655,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>344.5</v>
+        <v>345.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -8740,7 +8740,7 @@
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="21">
         <f>AVERAGE(H4:H42)</f>
-        <v>8.8333333333333339</v>
+        <v>8.8589743589743595</v>
       </c>
       <c r="B6" s="15">
         <v>1.5</v>
@@ -9900,7 +9900,7 @@
         <v>0.5</v>
       </c>
       <c r="E42" s="17">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="F42" s="17">
         <v>0</v>
@@ -9910,7 +9910,7 @@
       </c>
       <c r="H42" s="1">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I42" s="24">
         <v>39</v>
@@ -10003,7 +10003,7 @@
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="19">
         <f>SUM(H39:H45)</f>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>

</xml_diff>

<commit_message>
Last meeting of the day
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845311E1-8A71-4651-9EB5-DC34BCF06D7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24267F60-7A4E-4AF5-93C0-5A9455EC37D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1030,7 +1030,7 @@
                   <c:v>61.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>64</c:v>
+                  <c:v>65.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>69.5</c:v>
@@ -1391,7 +1391,7 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>10.25</c:v>
+                  <c:v>11.75</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>0</c:v>
@@ -2131,7 +2131,7 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>10.25</c:v>
+                  <c:v>11.75</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>0</c:v>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>64</c:v>
+                  <c:v>65.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4537,7 +4537,7 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2.5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8589,8 +8589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8657,7 +8657,7 @@
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>64</v>
+        <v>65.5</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
@@ -8673,7 +8673,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>355.75</v>
+        <v>357.25</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -8757,8 +8757,8 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="21">
-        <f>AVERAGE(H4:H42)</f>
-        <v>8.8589743589743595</v>
+        <f>AVERAGE(H4:H43)</f>
+        <v>8.9312500000000004</v>
       </c>
       <c r="B6" s="15">
         <v>1.5</v>
@@ -9948,7 +9948,7 @@
         <v>0.25</v>
       </c>
       <c r="D43" s="17">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="E43" s="17">
         <v>0.5</v>
@@ -9961,7 +9961,7 @@
       </c>
       <c r="H43" s="1">
         <f t="shared" si="1"/>
-        <v>10.25</v>
+        <v>11.75</v>
       </c>
       <c r="I43" s="24">
         <v>40</v>
@@ -10033,7 +10033,7 @@
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="19">
         <f>SUM(H39:H45)</f>
-        <v>58.25</v>
+        <v>59.75</v>
       </c>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>

</xml_diff>

<commit_message>
I need to stop
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24267F60-7A4E-4AF5-93C0-5A9455EC37D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32EDBC26-5555-418B-A31E-5876150530FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1030,7 +1030,7 @@
                   <c:v>61.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>65.5</c:v>
+                  <c:v>66.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>69.5</c:v>
@@ -1391,7 +1391,7 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>11.75</c:v>
+                  <c:v>12.75</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>0</c:v>
@@ -2131,7 +2131,7 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>11.75</c:v>
+                  <c:v>12.75</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>0</c:v>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>65.5</c:v>
+                  <c:v>66.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4537,7 +4537,7 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8589,8 +8589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8657,7 +8657,7 @@
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>65.5</v>
+        <v>66.5</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
@@ -8673,7 +8673,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>357.25</v>
+        <v>358.25</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -8758,7 +8758,7 @@
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="21">
         <f>AVERAGE(H4:H43)</f>
-        <v>8.9312500000000004</v>
+        <v>8.9562500000000007</v>
       </c>
       <c r="B6" s="15">
         <v>1.5</v>
@@ -9948,7 +9948,7 @@
         <v>0.25</v>
       </c>
       <c r="D43" s="17">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E43" s="17">
         <v>0.5</v>
@@ -9961,7 +9961,7 @@
       </c>
       <c r="H43" s="1">
         <f t="shared" si="1"/>
-        <v>11.75</v>
+        <v>12.75</v>
       </c>
       <c r="I43" s="24">
         <v>40</v>
@@ -10033,7 +10033,7 @@
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="19">
         <f>SUM(H39:H45)</f>
-        <v>59.75</v>
+        <v>60.75</v>
       </c>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>

</xml_diff>

<commit_message>
That's the plan anyway
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A2EC27-A028-4A1B-9C15-3E29960CEF73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4244F4-CA04-4094-8DE2-6777B2E0AFFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1030,7 +1030,7 @@
                   <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>77.5</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>74</c:v>
@@ -1406,7 +1406,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>0</c:v>
@@ -2146,7 +2146,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>0</c:v>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>77.5</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4576,7 +4576,7 @@
                   <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8738,7 +8738,7 @@
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>77.5</v>
+        <v>78</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
@@ -8754,7 +8754,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>399</v>
+        <v>399.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -8838,8 +8838,8 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="21">
-        <f>AVERAGE(H4:H46)</f>
-        <v>9</v>
+        <f>AVERAGE(H4:H47)</f>
+        <v>9.0227272727272734</v>
       </c>
       <c r="B6" s="15">
         <v>1.5</v>
@@ -10185,7 +10185,7 @@
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
       <c r="D48" s="15">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E48" s="15">
         <v>0.5</v>
@@ -10196,7 +10196,7 @@
       </c>
       <c r="H48" s="1">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="I48" s="24">
         <v>45</v>
@@ -10307,7 +10307,7 @@
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="14">
         <f>SUM(H46:H52)</f>
-        <v>24</v>
+        <v>24.5</v>
       </c>
       <c r="B54" s="17"/>
       <c r="C54" s="17"/>

</xml_diff>

<commit_message>
All I see our projects
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B9318B-2013-4D29-88CE-0AC6742C9F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{483757A5-A972-4339-B48F-DF324159BAEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1027,13 +1027,13 @@
                   <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>67.5</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>78</c:v>
+                  <c:v>79.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>74.5</c:v>
+                  <c:v>75.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1406,7 +1406,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>0</c:v>
@@ -2146,7 +2146,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>0</c:v>
@@ -3218,7 +3218,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>67.5</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>78</c:v>
+                  <c:v>79.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3470,7 +3470,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>74.5</c:v>
+                  <c:v>75.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4379,7 +4379,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4582,7 +4582,7 @@
                   <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4785,7 +4785,7 @@
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8680,7 +8680,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8743,15 +8743,15 @@
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
-        <v>67.5</v>
+        <v>68</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>78</v>
+        <v>79.5</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>74.5</v>
+        <v>75.5</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -8763,7 +8763,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -10195,13 +10195,13 @@
         <v>0.5</v>
       </c>
       <c r="C48" s="15">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D48" s="15">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E48" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F48" s="15">
         <v>0</v>
@@ -10211,7 +10211,7 @@
       </c>
       <c r="H48" s="1">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I48" s="24">
         <v>45</v>
@@ -10322,7 +10322,7 @@
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="14">
         <f>SUM(H46:H52)</f>
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B54" s="17"/>
       <c r="C54" s="17"/>

</xml_diff>

<commit_message>
Project plan setup finalized
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9038C4B7-60C8-4014-9643-E380DC9EAAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65486763-D999-4A2C-8F1E-91F780FA5B8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1030,7 +1030,7 @@
                   <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>83</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>78.5</c:v>
@@ -1409,7 +1409,7 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>5.5</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="46">
                   <c:v>0</c:v>
@@ -2149,7 +2149,7 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>5.5</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="46">
                   <c:v>0</c:v>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>83</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4585,7 +4585,7 @@
                   <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1.5</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8759,7 +8759,7 @@
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
@@ -8775,7 +8775,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>414.5</v>
+        <v>415.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -10236,7 +10236,7 @@
       <c r="B49" s="15"/>
       <c r="C49" s="15"/>
       <c r="D49" s="15">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="E49" s="15">
         <v>1</v>
@@ -10249,7 +10249,7 @@
       </c>
       <c r="H49" s="1">
         <f t="shared" si="2"/>
-        <v>5.5</v>
+        <v>6.5</v>
       </c>
       <c r="I49" s="24">
         <v>46</v>
@@ -10342,7 +10342,7 @@
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="14">
         <f>SUM(H46:H52)</f>
-        <v>39.5</v>
+        <v>40.5</v>
       </c>
       <c r="B54" s="17"/>
       <c r="C54" s="17"/>

</xml_diff>

<commit_message>
We're in the end game now
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98CBD84-10EA-49B7-9DB6-3F8F83AB4AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED4BDE7-A1D9-4D16-8090-6CF757C4C98A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1030,10 +1030,10 @@
                   <c:v>70.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>97.5</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>93.5</c:v>
+                  <c:v>94.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1427,7 +1427,7 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>7</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="52">
                   <c:v>0</c:v>
@@ -2167,7 +2167,7 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>7</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="52">
                   <c:v>0</c:v>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>97.5</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3470,7 +3470,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>93.5</c:v>
+                  <c:v>94.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4641,6 +4641,9 @@
                 <c:pt idx="50">
                   <c:v>0.5</c:v>
                 </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4863,7 +4866,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2.5</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8800,7 +8803,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8867,11 +8870,11 @@
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>97.5</v>
+        <v>98</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>93.5</v>
+        <v>94.5</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -8883,7 +8886,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>479</v>
+        <v>480.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -10538,9 +10541,11 @@
         <v>0.5</v>
       </c>
       <c r="C55" s="17"/>
-      <c r="D55" s="17"/>
+      <c r="D55" s="17">
+        <v>0.5</v>
+      </c>
       <c r="E55" s="17">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="F55" s="17">
         <v>0</v>
@@ -10550,7 +10555,7 @@
       </c>
       <c r="H55" s="1">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>8.5</v>
       </c>
       <c r="I55" s="24">
         <v>52</v>
@@ -10661,7 +10666,7 @@
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="19">
         <f>SUM(H53:H59)</f>
-        <v>27</v>
+        <v>28.5</v>
       </c>
       <c r="B61" s="15"/>
       <c r="C61" s="15"/>

</xml_diff>

<commit_message>
we march till dawn
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3297EFC5-311C-499F-A0B4-EC5499CB3A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC67CBC8-867C-434C-90E0-0C4A56F77598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1024,22 +1024,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>84</c:v>
+                  <c:v>84.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>110</c:v>
+                  <c:v>110.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>97.5</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>152.5</c:v>
+                  <c:v>153</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1442,7 +1442,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>8.5</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>0</c:v>
@@ -2182,7 +2182,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>8.5</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>0</c:v>
@@ -3092,7 +3092,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>84</c:v>
+                  <c:v>84.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>110</c:v>
+                  <c:v>110.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3470,7 +3470,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>97.5</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3722,7 +3722,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>152.5</c:v>
+                  <c:v>153</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4212,7 +4212,7 @@
                   <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.25</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4690,7 +4690,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4929,7 +4929,7 @@
                   <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.25</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5407,7 +5407,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8896,7 +8896,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8955,7 +8955,7 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>84</v>
+        <v>84.5</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
@@ -8963,11 +8963,11 @@
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>110</v>
+        <v>110.5</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>97.5</v>
+        <v>98</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -8975,11 +8975,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>152.5</v>
+        <v>153</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -9064,7 +9064,7 @@
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="21">
         <f>AVERAGE(H4:H60)</f>
-        <v>9.4035087719298254</v>
+        <v>9.4385964912280702</v>
       </c>
       <c r="B6" s="15">
         <v>1.5</v>
@@ -10790,26 +10790,26 @@
         <v>26</v>
       </c>
       <c r="B60" s="15">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="C60" s="15">
         <v>6</v>
       </c>
       <c r="D60" s="15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E60" s="15">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="F60" s="15">
         <v>0</v>
       </c>
       <c r="G60" s="15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="H60" s="1">
         <f t="shared" si="4"/>
-        <v>8.5</v>
+        <v>10.5</v>
       </c>
       <c r="I60" s="24">
         <v>57</v>
@@ -10960,7 +10960,7 @@
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="14">
         <f>SUM(H60:H66)</f>
-        <v>8.5</v>
+        <v>10.5</v>
       </c>
       <c r="B68" s="17"/>
       <c r="C68" s="17"/>

</xml_diff>

<commit_message>
work through next hour
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8446C8-0145-45A2-AC3A-3893AB258072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6C038A-BE61-452A-98F0-D0DDFC98D0D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1024,16 +1024,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>88</c:v>
+                  <c:v>92.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>92</c:v>
+                  <c:v>92.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>111.5</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98</c:v>
+                  <c:v>98.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1445,7 +1445,7 @@
                   <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>0</c:v>
@@ -2185,7 +2185,7 @@
                   <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>0</c:v>
@@ -3092,7 +3092,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>88</c:v>
+                  <c:v>92.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3218,7 +3218,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>92</c:v>
+                  <c:v>92.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>111.5</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3470,7 +3470,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>98</c:v>
+                  <c:v>98.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4215,7 +4215,7 @@
                   <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>3.5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4456,6 +4456,9 @@
                 <c:pt idx="56">
                   <c:v>6</c:v>
                 </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4695,6 +4698,9 @@
                 <c:pt idx="56">
                   <c:v>2.5</c:v>
                 </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4934,6 +4940,9 @@
                 <c:pt idx="56">
                   <c:v>0.75</c:v>
                 </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5171,6 +5180,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="57">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -8902,7 +8914,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G62" sqref="G62"/>
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8961,19 +8973,19 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>88</v>
+        <v>92.5</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
-        <v>92</v>
+        <v>92.5</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>111.5</v>
+        <v>112</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>98</v>
+        <v>98.5</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -8985,7 +8997,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>543</v>
+        <v>549</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -10830,18 +10842,26 @@
         <v>75.5</v>
       </c>
       <c r="B61" s="15">
-        <v>3.5</v>
-      </c>
-      <c r="C61" s="15"/>
-      <c r="D61" s="15"/>
-      <c r="E61" s="15"/>
-      <c r="F61" s="15"/>
+        <v>8</v>
+      </c>
+      <c r="C61" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="D61" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="E61" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F61" s="15">
+        <v>0</v>
+      </c>
       <c r="G61" s="15">
         <v>0.5</v>
       </c>
       <c r="H61" s="1">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="I61" s="24">
         <v>58</v>
@@ -10970,7 +10990,7 @@
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="14">
         <f>SUM(H60:H66)</f>
-        <v>15.5</v>
+        <v>21.5</v>
       </c>
       <c r="B68" s="17"/>
       <c r="C68" s="17"/>

</xml_diff>

<commit_message>
We code till dawn
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6C038A-BE61-452A-98F0-D0DDFC98D0D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454A7473-36DB-4C22-8DE3-A672EF902A58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1024,13 +1024,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>92.5</c:v>
+                  <c:v>94.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>92.5</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>112</c:v>
+                  <c:v>112.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>98.5</c:v>
@@ -1039,7 +1039,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>153.5</c:v>
+                  <c:v>154</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1445,7 +1445,7 @@
                   <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>10</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>0</c:v>
@@ -2185,7 +2185,7 @@
                   <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>10</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>0</c:v>
@@ -3092,7 +3092,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>92.5</c:v>
+                  <c:v>94.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3218,7 +3218,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>92.5</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>112</c:v>
+                  <c:v>112.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3722,7 +3722,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>153.5</c:v>
+                  <c:v>154</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4215,7 +4215,7 @@
                   <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4457,7 +4457,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4699,7 +4699,7 @@
                   <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5425,7 +5425,7 @@
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8913,7 +8913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
@@ -8973,15 +8973,15 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>92.5</v>
+        <v>94.5</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
-        <v>92.5</v>
+        <v>93</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>112</v>
+        <v>112.5</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
@@ -8993,11 +8993,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>153.5</v>
+        <v>154</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>549</v>
+        <v>552.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -10842,13 +10842,13 @@
         <v>75.5</v>
       </c>
       <c r="B61" s="15">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C61" s="15">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D61" s="15">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E61" s="15">
         <v>0.5</v>
@@ -10857,11 +10857,11 @@
         <v>0</v>
       </c>
       <c r="G61" s="15">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H61" s="1">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>13.5</v>
       </c>
       <c r="I61" s="24">
         <v>58</v>
@@ -10990,7 +10990,7 @@
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="14">
         <f>SUM(H60:H66)</f>
-        <v>21.5</v>
+        <v>25</v>
       </c>
       <c r="B68" s="17"/>
       <c r="C68" s="17"/>

</xml_diff>

<commit_message>
This is where the fun begins
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454A7473-36DB-4C22-8DE3-A672EF902A58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13267659-A60C-4D53-909F-5C6863918CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1024,22 +1024,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>94.5</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>93</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>112.5</c:v>
+                  <c:v>113</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98.5</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>154</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1448,7 +1448,7 @@
                   <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="59">
                   <c:v>0</c:v>
@@ -2188,7 +2188,7 @@
                   <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="59">
                   <c:v>0</c:v>
@@ -3092,7 +3092,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>94.5</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3218,7 +3218,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>93</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>112.5</c:v>
+                  <c:v>113</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3470,7 +3470,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>98.5</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3722,7 +3722,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>154</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4217,6 +4217,9 @@
                 <c:pt idx="57">
                   <c:v>10</c:v>
                 </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4459,6 +4462,9 @@
                 <c:pt idx="57">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="58">
+                  <c:v>2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4701,6 +4707,9 @@
                 <c:pt idx="57">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4943,6 +4952,9 @@
                 <c:pt idx="57">
                   <c:v>0.5</c:v>
                 </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5183,6 +5195,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -5425,6 +5440,9 @@
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="57">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="58">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -8913,8 +8931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8973,19 +8991,19 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>94.5</v>
+        <v>95</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>112.5</v>
+        <v>113</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>98.5</v>
+        <v>99</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -8993,11 +9011,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>552.5</v>
+        <v>557</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -10871,15 +10889,27 @@
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B62" s="15"/>
-      <c r="C62" s="15"/>
-      <c r="D62" s="15"/>
-      <c r="E62" s="15"/>
-      <c r="F62" s="15"/>
-      <c r="G62" s="15"/>
+      <c r="B62" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="C62" s="15">
+        <v>2</v>
+      </c>
+      <c r="D62" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="E62" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F62" s="15">
+        <v>0</v>
+      </c>
+      <c r="G62" s="15">
+        <v>1</v>
+      </c>
       <c r="H62" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="I62" s="24">
         <v>59</v>
@@ -10990,7 +11020,7 @@
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="14">
         <f>SUM(H60:H66)</f>
-        <v>25</v>
+        <v>29.5</v>
       </c>
       <c r="B68" s="17"/>
       <c r="C68" s="17"/>

</xml_diff>

<commit_message>
work through next couple hours
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13267659-A60C-4D53-909F-5C6863918CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0E993B-1289-4B20-A483-6955C93D4D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1027,7 +1027,7 @@
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>95</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>113</c:v>
@@ -1039,7 +1039,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>155</c:v>
+                  <c:v>155.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1448,7 +1448,7 @@
                   <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>4.5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="59">
                   <c:v>0</c:v>
@@ -2188,7 +2188,7 @@
                   <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>4.5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="59">
                   <c:v>0</c:v>
@@ -3218,7 +3218,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>95</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3722,7 +3722,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>155</c:v>
+                  <c:v>155.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4463,7 +4463,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5443,7 +5443,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8932,7 +8932,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8995,7 +8995,7 @@
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
@@ -9011,11 +9011,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>155</v>
+        <v>155.5</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>557</v>
+        <v>558.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -10893,7 +10893,7 @@
         <v>0.5</v>
       </c>
       <c r="C62" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D62" s="15">
         <v>0.5</v>
@@ -10905,11 +10905,11 @@
         <v>0</v>
       </c>
       <c r="G62" s="15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="H62" s="1">
         <f t="shared" si="4"/>
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="I62" s="24">
         <v>59</v>
@@ -11020,7 +11020,7 @@
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="14">
         <f>SUM(H60:H66)</f>
-        <v>29.5</v>
+        <v>31</v>
       </c>
       <c r="B68" s="17"/>
       <c r="C68" s="17"/>

</xml_diff>

<commit_message>
lots of work to do
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0E993B-1289-4B20-A483-6955C93D4D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC74B87-E71C-4CFF-8CD8-CA9DA57C9B31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1024,13 +1024,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>95</c:v>
+                  <c:v>95.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>96</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>113</c:v>
+                  <c:v>115.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>99</c:v>
@@ -1039,7 +1039,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>155.5</c:v>
+                  <c:v>156</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1448,7 +1448,7 @@
                   <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>6</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="59">
                   <c:v>0</c:v>
@@ -2188,7 +2188,7 @@
                   <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>6</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="59">
                   <c:v>0</c:v>
@@ -3092,7 +3092,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>95</c:v>
+                  <c:v>95.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3218,7 +3218,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>96</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>113</c:v>
+                  <c:v>115.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3722,7 +3722,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>155.5</c:v>
+                  <c:v>156</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4218,7 +4218,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4463,7 +4463,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4708,7 +4708,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5443,7 +5443,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1.5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8932,7 +8932,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+      <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8991,15 +8991,15 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>95</v>
+        <v>95.5</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>113</v>
+        <v>115.5</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
@@ -9011,11 +9011,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>155.5</v>
+        <v>156</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>558.5</v>
+        <v>565</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -10890,13 +10890,13 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B62" s="15">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C62" s="15">
+        <v>6</v>
+      </c>
+      <c r="D62" s="15">
         <v>3</v>
-      </c>
-      <c r="D62" s="15">
-        <v>0.5</v>
       </c>
       <c r="E62" s="15">
         <v>0.5</v>
@@ -10905,11 +10905,11 @@
         <v>0</v>
       </c>
       <c r="G62" s="15">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="H62" s="1">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>12.5</v>
       </c>
       <c r="I62" s="24">
         <v>59</v>
@@ -11020,7 +11020,7 @@
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="14">
         <f>SUM(H60:H66)</f>
-        <v>31</v>
+        <v>37.5</v>
       </c>
       <c r="B68" s="17"/>
       <c r="C68" s="17"/>

</xml_diff>

<commit_message>
can't stop won't stop
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC74B87-E71C-4CFF-8CD8-CA9DA57C9B31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCF74A1-4DDB-4685-9086-1802AC47DB03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1024,22 +1024,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>95.5</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>99</c:v>
+                  <c:v>99.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>115.5</c:v>
+                  <c:v>116.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>99</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>156</c:v>
+                  <c:v>157</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1448,10 +1448,10 @@
                   <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>12.5</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="60">
                   <c:v>0</c:v>
@@ -2188,10 +2188,10 @@
                   <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>12.5</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="60">
                   <c:v>0</c:v>
@@ -3092,7 +3092,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>95.5</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3218,7 +3218,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>99</c:v>
+                  <c:v>99.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>115.5</c:v>
+                  <c:v>116.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3470,7 +3470,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>99</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3722,7 +3722,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>156</c:v>
+                  <c:v>157</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4220,6 +4220,9 @@
                 <c:pt idx="58">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4465,6 +4468,9 @@
                 <c:pt idx="58">
                   <c:v>6</c:v>
                 </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4708,7 +4714,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>3</c:v>
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4955,6 +4964,9 @@
                 <c:pt idx="58">
                   <c:v>0.5</c:v>
                 </c:pt>
+                <c:pt idx="59">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5198,6 +5210,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -5444,6 +5459,9 @@
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8931,8 +8949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8991,19 +9009,19 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>95.5</v>
+        <v>96</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
-        <v>99</v>
+        <v>99.5</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>115.5</v>
+        <v>116.5</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -9011,11 +9029,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -10896,7 +10914,7 @@
         <v>6</v>
       </c>
       <c r="D62" s="15">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="E62" s="15">
         <v>0.5</v>
@@ -10909,7 +10927,7 @@
       </c>
       <c r="H62" s="1">
         <f t="shared" si="4"/>
-        <v>12.5</v>
+        <v>13</v>
       </c>
       <c r="I62" s="24">
         <v>59</v>
@@ -10919,15 +10937,27 @@
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B63" s="15"/>
-      <c r="C63" s="15"/>
-      <c r="D63" s="15"/>
-      <c r="E63" s="15"/>
-      <c r="F63" s="15"/>
-      <c r="G63" s="15"/>
+      <c r="B63" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="C63" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="D63" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="E63" s="15">
+        <v>1</v>
+      </c>
+      <c r="F63" s="15">
+        <v>0</v>
+      </c>
+      <c r="G63" s="15">
+        <v>1</v>
+      </c>
       <c r="H63" s="1">
         <f t="shared" ref="H63:H68" si="5">SUM(B63:G63)</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="I63" s="24">
         <v>60</v>
@@ -11020,7 +11050,7 @@
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="14">
         <f>SUM(H60:H66)</f>
-        <v>37.5</v>
+        <v>41.5</v>
       </c>
       <c r="B68" s="17"/>
       <c r="C68" s="17"/>

</xml_diff>

<commit_message>
Shall I work more?
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB01F634-D2E7-4871-A168-528FA4999F19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573C1326-FFE8-41B0-B6B1-BC603E409ABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1033,7 +1033,7 @@
                   <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>116</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1454,7 +1454,7 @@
                   <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>14</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="61">
                   <c:v>0</c:v>
@@ -2194,7 +2194,7 @@
                   <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>14</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="61">
                   <c:v>0</c:v>
@@ -3470,7 +3470,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>116</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4974,7 +4974,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8962,7 +8962,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9033,7 +9033,7 @@
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -9045,7 +9045,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -10990,7 +10990,7 @@
         <v>2.5</v>
       </c>
       <c r="E64" s="15">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F64" s="15">
         <v>0</v>
@@ -10998,7 +10998,7 @@
       <c r="G64" s="15"/>
       <c r="H64" s="1">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I64" s="24">
         <v>61</v>
@@ -11070,7 +11070,7 @@
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="14">
         <f>SUM(H60:H66)</f>
-        <v>63.5</v>
+        <v>64.5</v>
       </c>
       <c r="B68" s="17"/>
       <c r="C68" s="17"/>

</xml_diff>

<commit_message>
morning work on bash and setup
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E403640B-11D5-4F6A-A0A6-D79C5C2BB853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6AE8264-9282-4341-8099-0BF38754E174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1024,22 +1024,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>109</c:v>
+                  <c:v>111</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>107</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>118</c:v>
+                  <c:v>118.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>162.5</c:v>
+                  <c:v>163</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1466,7 +1466,7 @@
                   <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>0</c:v>
@@ -2206,7 +2206,7 @@
                   <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>0</c:v>
@@ -3092,7 +3092,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>109</c:v>
+                  <c:v>111</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3218,7 +3218,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>107</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3470,7 +3470,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>118</c:v>
+                  <c:v>118.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3722,7 +3722,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>162.5</c:v>
+                  <c:v>163</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4235,6 +4235,9 @@
                 <c:pt idx="63">
                   <c:v>11</c:v>
                 </c:pt>
+                <c:pt idx="64">
+                  <c:v>2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4495,6 +4498,9 @@
                 <c:pt idx="63">
                   <c:v>0.5</c:v>
                 </c:pt>
+                <c:pt idx="64">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5015,6 +5021,9 @@
                 <c:pt idx="63">
                   <c:v>0.5</c:v>
                 </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5533,6 +5542,9 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="63">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="64">
                   <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
@@ -9021,8 +9033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9081,11 +9093,11 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
@@ -9093,7 +9105,7 @@
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>118</v>
+        <v>118.5</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -9101,11 +9113,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>162.5</v>
+        <v>163</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>620.5</v>
+        <v>624.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -11172,15 +11184,23 @@
         <f>SUM(H60:H66)</f>
         <v>78.5</v>
       </c>
-      <c r="B68" s="17"/>
-      <c r="C68" s="17"/>
+      <c r="B68" s="17">
+        <v>2</v>
+      </c>
+      <c r="C68" s="17">
+        <v>1</v>
+      </c>
       <c r="D68" s="17"/>
-      <c r="E68" s="17"/>
+      <c r="E68" s="17">
+        <v>0.5</v>
+      </c>
       <c r="F68" s="17"/>
-      <c r="G68" s="17"/>
+      <c r="G68" s="17">
+        <v>0.5</v>
+      </c>
       <c r="H68" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I68" s="24">
         <v>65</v>
@@ -11306,7 +11326,7 @@
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="19">
         <f>SUM(H67:H73)</f>
-        <v>14.5</v>
+        <v>18.5</v>
       </c>
       <c r="B75" s="15"/>
       <c r="C75" s="15"/>

</xml_diff>

<commit_message>
more documentation and pres setup
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DA0FC3-87E6-4597-836B-5AC4F29BB27C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078C17FF-7E06-4E11-A02B-2787F3F596BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1030,7 +1030,7 @@
                   <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>125.5</c:v>
+                  <c:v>126.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>118.5</c:v>
@@ -1466,7 +1466,7 @@
                   <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>5.5</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>0</c:v>
@@ -2206,7 +2206,7 @@
                   <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>5.5</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>0</c:v>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>125.5</c:v>
+                  <c:v>126.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4762,7 +4762,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1.5</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9104,7 +9104,7 @@
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>125.5</v>
+        <v>126.5</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
@@ -9120,7 +9120,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -11194,7 +11194,7 @@
         <v>1</v>
       </c>
       <c r="D68" s="17">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="E68" s="17">
         <v>0.5</v>
@@ -11205,7 +11205,7 @@
       </c>
       <c r="H68" s="1">
         <f t="shared" si="5"/>
-        <v>5.5</v>
+        <v>6.5</v>
       </c>
       <c r="I68" s="24">
         <v>65</v>
@@ -11331,7 +11331,7 @@
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="19">
         <f>SUM(H67:H73)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B75" s="15"/>
       <c r="C75" s="15"/>

</xml_diff>

<commit_message>
setup and clerical work
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEAD5175-79DA-415C-BC0F-065B04EB25DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDD7A1F-6313-453C-BF32-7FF77842C24B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1024,16 +1024,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>113</c:v>
+                  <c:v>113.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>109</c:v>
+                  <c:v>109.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>139</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>125.5</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1475,7 +1475,7 @@
                   <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>3.5</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="68">
                   <c:v>0</c:v>
@@ -2215,7 +2215,7 @@
                   <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>3.5</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="68">
                   <c:v>0</c:v>
@@ -3092,7 +3092,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>113</c:v>
+                  <c:v>113.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3218,7 +3218,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>109</c:v>
+                  <c:v>109.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3470,7 +3470,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>125.5</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4244,6 +4244,9 @@
                 <c:pt idx="66">
                   <c:v>1.5</c:v>
                 </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4513,6 +4516,9 @@
                 <c:pt idx="66">
                   <c:v>0.5</c:v>
                 </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5053,6 +5059,9 @@
                 </c:pt>
                 <c:pt idx="66">
                   <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9082,7 +9091,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+      <selection activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9141,11 +9150,11 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>113</v>
+        <v>113.5</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
-        <v>109</v>
+        <v>109.5</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
@@ -9153,7 +9162,7 @@
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>125.5</v>
+        <v>126</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -9165,7 +9174,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>656</v>
+        <v>657.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -11322,19 +11331,25 @@
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B71" s="17"/>
-      <c r="C71" s="17"/>
+      <c r="B71" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="C71" s="17">
+        <v>0.5</v>
+      </c>
       <c r="D71" s="17">
         <v>3</v>
       </c>
-      <c r="E71" s="17"/>
+      <c r="E71" s="17">
+        <v>0.5</v>
+      </c>
       <c r="F71" s="17"/>
       <c r="G71" s="17">
         <v>0.5</v>
       </c>
       <c r="H71" s="1">
         <f t="shared" si="6"/>
-        <v>3.5</v>
+        <v>5</v>
       </c>
       <c r="I71" s="24">
         <v>68</v>
@@ -11406,7 +11421,7 @@
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="19">
         <f>SUM(H67:H73)</f>
-        <v>50</v>
+        <v>51.5</v>
       </c>
       <c r="B75" s="15"/>
       <c r="C75" s="15"/>

</xml_diff>

<commit_message>
I know I know nothing
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522711A2-E64B-4D36-B4CF-BB9462AC9179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E429EA-37FE-48CC-AB3D-55BD34902424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1027,10 +1027,10 @@
                   <c:v>119.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>112.5</c:v>
+                  <c:v>114.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>146</c:v>
+                  <c:v>146.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>130.5</c:v>
@@ -1484,7 +1484,7 @@
                   <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>7.5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>0</c:v>
@@ -2224,7 +2224,7 @@
                   <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>7.5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>0</c:v>
@@ -3218,7 +3218,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>112.5</c:v>
+                  <c:v>114.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>146</c:v>
+                  <c:v>146.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4535,7 +4535,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.5</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4816,7 +4816,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>2</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9148,7 +9148,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9211,11 +9211,11 @@
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
-        <v>112.5</v>
+        <v>114.5</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>146</v>
+        <v>146.5</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
@@ -9231,7 +9231,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>681</v>
+        <v>683.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -11488,10 +11488,10 @@
         <v>3.5</v>
       </c>
       <c r="C74" s="15">
-        <v>0.5</v>
+        <v>2.5</v>
       </c>
       <c r="D74" s="15">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="E74" s="15">
         <v>0.5</v>
@@ -11504,7 +11504,7 @@
       </c>
       <c r="H74" s="1">
         <f t="shared" si="6"/>
-        <v>7.5</v>
+        <v>10</v>
       </c>
       <c r="I74" s="24">
         <v>71</v>
@@ -11655,7 +11655,7 @@
     <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" s="14">
         <f>SUM(H74:H80)</f>
-        <v>7.5</v>
+        <v>10</v>
       </c>
       <c r="B82" s="17"/>
       <c r="C82" s="17"/>

</xml_diff>

<commit_message>
mostly done on each
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA1DFB7-327D-42F1-AFD5-BBFC98F473B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341422FB-2374-4C26-B128-E771C59D9C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1027,7 +1027,7 @@
                   <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>115</c:v>
+                  <c:v>115.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>146.5</c:v>
@@ -1484,7 +1484,7 @@
                   <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>13</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>0</c:v>
@@ -2224,7 +2224,7 @@
                   <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>13</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>0</c:v>
@@ -3218,7 +3218,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>115</c:v>
+                  <c:v>115.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4535,7 +4535,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>3</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9148,7 +9148,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9211,7 +9211,7 @@
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
-        <v>115</v>
+        <v>115.5</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
@@ -9231,7 +9231,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>686.5</v>
+        <v>687</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -11488,7 +11488,7 @@
         <v>6</v>
       </c>
       <c r="C74" s="15">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="D74" s="15">
         <v>2.5</v>
@@ -11504,7 +11504,7 @@
       </c>
       <c r="H74" s="1">
         <f t="shared" si="6"/>
-        <v>13</v>
+        <v>13.5</v>
       </c>
       <c r="I74" s="24">
         <v>71</v>
@@ -11655,7 +11655,7 @@
     <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" s="14">
         <f>SUM(H74:H80)</f>
-        <v>13</v>
+        <v>13.5</v>
       </c>
       <c r="B82" s="17"/>
       <c r="C82" s="17"/>

</xml_diff>

<commit_message>
Logistics and follow up
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341422FB-2374-4C26-B128-E771C59D9C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4D2EAA-819F-4B4C-914B-B7B494340376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1024,13 +1024,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>122</c:v>
+                  <c:v>123.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>115.5</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>146.5</c:v>
+                  <c:v>147</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>130.5</c:v>
@@ -1039,7 +1039,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>172.5</c:v>
+                  <c:v>174.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1487,7 +1487,7 @@
                   <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="72">
                   <c:v>0</c:v>
@@ -2227,7 +2227,7 @@
                   <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="72">
                   <c:v>0</c:v>
@@ -3092,7 +3092,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>122</c:v>
+                  <c:v>123.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3218,7 +3218,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>115.5</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>146.5</c:v>
+                  <c:v>147</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3722,7 +3722,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>172.5</c:v>
+                  <c:v>174.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4256,6 +4256,9 @@
                 <c:pt idx="70">
                   <c:v>6</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>1.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4537,6 +4540,9 @@
                 <c:pt idx="70">
                   <c:v>3.5</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4818,6 +4824,9 @@
                 <c:pt idx="70">
                   <c:v>2.5</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5380,6 +5389,9 @@
                 <c:pt idx="70">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5660,6 +5672,9 @@
                 </c:pt>
                 <c:pt idx="70">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9147,8 +9162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9207,15 +9222,15 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>122</v>
+        <v>123.5</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
-        <v>115.5</v>
+        <v>116</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>146.5</v>
+        <v>147</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
@@ -9227,11 +9242,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>172.5</v>
+        <v>174.5</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>687</v>
+        <v>691.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -11518,15 +11533,25 @@
         <f>SUM(H67:H73)</f>
         <v>67.5</v>
       </c>
-      <c r="B75" s="15"/>
-      <c r="C75" s="15"/>
-      <c r="D75" s="15"/>
+      <c r="B75" s="15">
+        <v>1.5</v>
+      </c>
+      <c r="C75" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="D75" s="15">
+        <v>0.5</v>
+      </c>
       <c r="E75" s="15"/>
-      <c r="F75" s="15"/>
-      <c r="G75" s="15"/>
+      <c r="F75" s="15">
+        <v>0</v>
+      </c>
+      <c r="G75" s="15">
+        <v>2</v>
+      </c>
       <c r="H75" s="1">
         <f t="shared" ref="H75:H80" si="7">SUM(B75:G75)</f>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="I75" s="24">
         <v>72</v>
@@ -11655,7 +11680,7 @@
     <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" s="14">
         <f>SUM(H74:H80)</f>
-        <v>13.5</v>
+        <v>18</v>
       </c>
       <c r="B82" s="17"/>
       <c r="C82" s="17"/>

</xml_diff>

<commit_message>
The pit of dispair
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBB5B28-D127-4AEF-99FA-0FC678399C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6554EA0-5547-4737-8B01-D0EA68DDA364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1027,7 +1027,7 @@
                   <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>116.5</c:v>
+                  <c:v>118.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>147</c:v>
@@ -1487,7 +1487,7 @@
                   <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="72">
                   <c:v>0</c:v>
@@ -2227,7 +2227,7 @@
                   <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="72">
                   <c:v>0</c:v>
@@ -3218,7 +3218,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>116.5</c:v>
+                  <c:v>118.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4541,7 +4541,7 @@
                   <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9166,7 +9166,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9229,7 +9229,7 @@
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
-        <v>116.5</v>
+        <v>118.5</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
@@ -9249,7 +9249,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -11540,7 +11540,7 @@
         <v>2</v>
       </c>
       <c r="C75" s="15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D75" s="15">
         <v>0.5</v>
@@ -11556,7 +11556,7 @@
       </c>
       <c r="H75" s="1">
         <f t="shared" ref="H75:H80" si="7">SUM(B75:G75)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I75" s="24">
         <v>72</v>
@@ -11685,7 +11685,7 @@
     <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" s="14">
         <f>SUM(H74:H80)</f>
-        <v>20.5</v>
+        <v>22.5</v>
       </c>
       <c r="B82" s="17"/>
       <c r="C82" s="17"/>

</xml_diff>

<commit_message>
progress so far plus class
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB02C17A-EA35-4C93-8CFB-96C32FF21F20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD06D51-9BE5-4446-9DB1-91E355D7FF65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1024,22 +1024,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>150</c:v>
+                  <c:v>150.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>130.5</c:v>
+                  <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>161.5</c:v>
+                  <c:v>164</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>159</c:v>
+                  <c:v>159.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>189.5</c:v>
+                  <c:v>192</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1514,7 +1514,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="81">
                   <c:v>0</c:v>
@@ -2254,7 +2254,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="81">
                   <c:v>0</c:v>
@@ -3092,7 +3092,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>150</c:v>
+                  <c:v>150.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3218,7 +3218,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>130.5</c:v>
+                  <c:v>131</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>161.5</c:v>
+                  <c:v>164</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3470,7 +3470,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>159</c:v>
+                  <c:v>159.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3722,7 +3722,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>189.5</c:v>
+                  <c:v>192</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4283,6 +4283,9 @@
                 <c:pt idx="79">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4591,6 +4594,9 @@
                 <c:pt idx="79">
                   <c:v>3</c:v>
                 </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4899,6 +4905,9 @@
                 <c:pt idx="79">
                   <c:v>2</c:v>
                 </c:pt>
+                <c:pt idx="80">
+                  <c:v>2.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5207,6 +5216,9 @@
                 <c:pt idx="79">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5513,6 +5525,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="79">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="80">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -5822,6 +5837,9 @@
                 </c:pt>
                 <c:pt idx="79">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9309,8 +9327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D84" sqref="D84"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G85" sqref="G85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9369,19 +9387,19 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>150</v>
+        <v>150.5</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
-        <v>130.5</v>
+        <v>131</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>161.5</v>
+        <v>164</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>159</v>
+        <v>159.5</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -9389,11 +9407,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>189.5</v>
+        <v>192</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>790.5</v>
+        <v>797</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -11963,15 +11981,27 @@
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B84" s="17"/>
-      <c r="C84" s="17"/>
-      <c r="D84" s="17"/>
-      <c r="E84" s="17"/>
-      <c r="F84" s="17"/>
-      <c r="G84" s="17"/>
+      <c r="B84" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="C84" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="D84" s="17">
+        <v>2.5</v>
+      </c>
+      <c r="E84" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="F84" s="17">
+        <v>0</v>
+      </c>
+      <c r="G84" s="17">
+        <v>2.5</v>
+      </c>
       <c r="H84" s="1">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="I84" s="24">
         <v>81</v>
@@ -12064,7 +12094,7 @@
     <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" s="19">
         <f>SUM(H81:H87)</f>
-        <v>33</v>
+        <v>39.5</v>
       </c>
       <c r="B89" s="15"/>
       <c r="C89" s="15"/>

</xml_diff>

<commit_message>
Don't have a planakin
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C062C45-240D-4033-95DB-178550AC7A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC64939-7146-42DF-B6F7-AD3D6D6BD600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1024,7 +1024,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>155</c:v>
+                  <c:v>157</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>137</c:v>
@@ -1526,7 +1526,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="85">
                   <c:v>0</c:v>
@@ -2266,7 +2266,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="85">
                   <c:v>0</c:v>
@@ -3092,7 +3092,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>155</c:v>
+                  <c:v>157</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4296,7 +4296,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9400,7 +9400,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E89" sqref="E89"/>
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9459,7 +9459,7 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
@@ -9483,7 +9483,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -12183,7 +12183,7 @@
         <v>22</v>
       </c>
       <c r="B88" s="15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C88" s="15">
         <v>1</v>
@@ -12202,7 +12202,7 @@
       </c>
       <c r="H88" s="1">
         <f t="shared" si="9"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I88" s="24">
         <v>85</v>
@@ -12353,7 +12353,7 @@
     <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" s="14">
         <f>SUM(H88:H94)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B96" s="17"/>
       <c r="C96" s="17"/>

</xml_diff>

<commit_message>
Should be working on something else
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC64939-7146-42DF-B6F7-AD3D6D6BD600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311FF816-13D3-4B31-9DE1-E68CFD2736B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1024,16 +1024,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>157</c:v>
+                  <c:v>158</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>137</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>177</c:v>
+                  <c:v>180.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>162.5</c:v>
+                  <c:v>163</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1526,7 +1526,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>8</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="85">
                   <c:v>0</c:v>
@@ -2266,7 +2266,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>8</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="85">
                   <c:v>0</c:v>
@@ -3092,7 +3092,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>157</c:v>
+                  <c:v>158</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>177</c:v>
+                  <c:v>180.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3470,7 +3470,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>162.5</c:v>
+                  <c:v>163</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4296,7 +4296,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4942,7 +4942,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>2</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5265,7 +5265,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9400,7 +9400,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+      <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9459,7 +9459,7 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
@@ -9467,11 +9467,11 @@
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>177</v>
+        <v>180.5</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>162.5</v>
+        <v>163</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -9483,7 +9483,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>832</v>
+        <v>837</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -12183,16 +12183,16 @@
         <v>22</v>
       </c>
       <c r="B88" s="15">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C88" s="15">
         <v>1</v>
       </c>
       <c r="D88" s="15">
-        <v>2</v>
+        <v>5.5</v>
       </c>
       <c r="E88" s="15">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F88" s="15">
         <v>0</v>
@@ -12202,7 +12202,7 @@
       </c>
       <c r="H88" s="1">
         <f t="shared" si="9"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="I88" s="24">
         <v>85</v>
@@ -12353,7 +12353,7 @@
     <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" s="14">
         <f>SUM(H88:H94)</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B96" s="17"/>
       <c r="C96" s="17"/>

</xml_diff>

<commit_message>
Not the most urgent
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311FF816-13D3-4B31-9DE1-E68CFD2736B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E578AAD9-934B-480F-B1B7-0D452CC56959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1030,7 +1030,7 @@
                   <c:v>137</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>180.5</c:v>
+                  <c:v>181.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>163</c:v>
@@ -1526,7 +1526,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>13</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="85">
                   <c:v>0</c:v>
@@ -2266,7 +2266,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>13</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="85">
                   <c:v>0</c:v>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>180.5</c:v>
+                  <c:v>181.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4942,7 +4942,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>5.5</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9467,7 +9467,7 @@
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>180.5</v>
+        <v>181.5</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
@@ -9483,7 +9483,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -12189,7 +12189,7 @@
         <v>1</v>
       </c>
       <c r="D88" s="15">
-        <v>5.5</v>
+        <v>6.5</v>
       </c>
       <c r="E88" s="15">
         <v>1</v>
@@ -12202,7 +12202,7 @@
       </c>
       <c r="H88" s="1">
         <f t="shared" si="9"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I88" s="24">
         <v>85</v>
@@ -12353,7 +12353,7 @@
     <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" s="14">
         <f>SUM(H88:H94)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B96" s="17"/>
       <c r="C96" s="17"/>

</xml_diff>

<commit_message>
It can't end here
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{343D800E-BC30-4FA5-9788-04BE3AF9161E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558F8A74-9723-4696-B0CD-5ACFEFDD8FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1024,22 +1024,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>163</c:v>
+                  <c:v>165</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>137.5</c:v>
+                  <c:v>138</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>183.5</c:v>
+                  <c:v>184.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>163.5</c:v>
+                  <c:v>164</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>198.5</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1529,7 +1529,7 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>7</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="86">
                   <c:v>0</c:v>
@@ -2269,7 +2269,7 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>7</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="86">
                   <c:v>0</c:v>
@@ -3092,7 +3092,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>163</c:v>
+                  <c:v>165</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3218,7 +3218,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>137.5</c:v>
+                  <c:v>138</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>183.5</c:v>
+                  <c:v>184.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3470,7 +3470,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>163.5</c:v>
+                  <c:v>164</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3722,7 +3722,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>198.5</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4299,7 +4299,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4625,7 +4625,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4951,7 +4951,7 @@
                   <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5277,7 +5277,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5927,6 +5927,9 @@
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9414,8 +9417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E90" sqref="E90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9474,19 +9477,19 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
-        <v>137.5</v>
+        <v>138</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>183.5</v>
+        <v>184.5</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>163.5</v>
+        <v>164</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -9494,11 +9497,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>198.5</v>
+        <v>200</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>846</v>
+        <v>851.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -12232,24 +12235,26 @@
         <v>66.5</v>
       </c>
       <c r="B89" s="15">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C89" s="15">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D89" s="15">
+        <v>2</v>
+      </c>
+      <c r="E89" s="15">
         <v>1</v>
       </c>
-      <c r="E89" s="15">
-        <v>0.5</v>
-      </c>
       <c r="F89" s="15">
         <v>0</v>
       </c>
-      <c r="G89" s="15"/>
+      <c r="G89" s="15">
+        <v>1.5</v>
+      </c>
       <c r="H89" s="1">
         <f t="shared" si="9"/>
-        <v>7</v>
+        <v>12.5</v>
       </c>
       <c r="I89" s="24">
         <v>86</v>
@@ -12378,7 +12383,7 @@
     <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" s="14">
         <f>SUM(H88:H94)</f>
-        <v>22</v>
+        <v>27.5</v>
       </c>
       <c r="B96" s="17"/>
       <c r="C96" s="17"/>

</xml_diff>

<commit_message>
The end of break
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03818759-08DE-4F95-A1B4-646E8DD78F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713394E4-E386-4142-B0FA-B1E1BC2BAE06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1024,22 +1024,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>169</c:v>
+                  <c:v>170.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>147</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>206.5</c:v>
+                  <c:v>210.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>169.5</c:v>
+                  <c:v>171.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>211.5</c:v>
+                  <c:v>215.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1556,13 +1556,13 @@
                   <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="97">
                   <c:v>0</c:v>
@@ -2296,13 +2296,13 @@
                   <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="97">
                   <c:v>0</c:v>
@@ -3092,7 +3092,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>169</c:v>
+                  <c:v>170.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>206.5</c:v>
+                  <c:v>210.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3470,7 +3470,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>169.5</c:v>
+                  <c:v>171.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3722,7 +3722,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>211.5</c:v>
+                  <c:v>215.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4325,6 +4325,15 @@
                 <c:pt idx="93">
                   <c:v>0.5</c:v>
                 </c:pt>
+                <c:pt idx="94">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4672,6 +4681,18 @@
                 <c:pt idx="92">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="93">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5022,6 +5043,15 @@
                 <c:pt idx="93">
                   <c:v>3</c:v>
                 </c:pt>
+                <c:pt idx="94">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5372,6 +5402,15 @@
                 <c:pt idx="93">
                   <c:v>0.5</c:v>
                 </c:pt>
+                <c:pt idx="94">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5720,6 +5759,15 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="93">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="96">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -6071,6 +6119,15 @@
                 </c:pt>
                 <c:pt idx="93">
                   <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9559,7 +9616,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F98" sqref="F98"/>
+      <selection activeCell="F101" sqref="F101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9618,7 +9675,7 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>169</v>
+        <v>170.5</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
@@ -9626,11 +9683,11 @@
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>206.5</v>
+        <v>210.5</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>169.5</v>
+        <v>171.5</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -9638,11 +9695,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>211.5</v>
+        <v>215.5</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>903.5</v>
+        <v>915</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -12631,7 +12688,9 @@
       <c r="B97" s="17">
         <v>0.5</v>
       </c>
-      <c r="C97" s="17"/>
+      <c r="C97" s="17">
+        <v>0</v>
+      </c>
       <c r="D97" s="17">
         <v>3</v>
       </c>
@@ -12656,15 +12715,27 @@
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B98" s="17"/>
-      <c r="C98" s="17"/>
-      <c r="D98" s="17"/>
-      <c r="E98" s="17"/>
-      <c r="F98" s="17"/>
-      <c r="G98" s="17"/>
+      <c r="B98" s="17">
+        <v>0</v>
+      </c>
+      <c r="C98" s="17">
+        <v>0</v>
+      </c>
+      <c r="D98" s="17">
+        <v>1</v>
+      </c>
+      <c r="E98" s="17">
+        <v>0</v>
+      </c>
+      <c r="F98" s="17">
+        <v>0</v>
+      </c>
+      <c r="G98" s="17">
+        <v>0</v>
+      </c>
       <c r="H98" s="1">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I98" s="24">
         <v>95</v>
@@ -12677,15 +12748,27 @@
       <c r="A99" t="s">
         <v>41</v>
       </c>
-      <c r="B99" s="17"/>
-      <c r="C99" s="17"/>
-      <c r="D99" s="17"/>
-      <c r="E99" s="17"/>
-      <c r="F99" s="17"/>
-      <c r="G99" s="17"/>
+      <c r="B99" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="C99" s="17">
+        <v>0</v>
+      </c>
+      <c r="D99" s="17">
+        <v>1</v>
+      </c>
+      <c r="E99" s="17">
+        <v>1</v>
+      </c>
+      <c r="F99" s="17">
+        <v>0</v>
+      </c>
+      <c r="G99" s="17">
+        <v>2</v>
+      </c>
       <c r="H99" s="1">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="I99" s="24">
         <v>96</v>
@@ -12698,15 +12781,27 @@
       <c r="A100" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B100" s="17"/>
-      <c r="C100" s="17"/>
-      <c r="D100" s="17"/>
-      <c r="E100" s="17"/>
-      <c r="F100" s="17"/>
-      <c r="G100" s="17"/>
+      <c r="B100" s="17">
+        <v>1</v>
+      </c>
+      <c r="C100" s="17">
+        <v>0</v>
+      </c>
+      <c r="D100" s="17">
+        <v>2</v>
+      </c>
+      <c r="E100" s="17">
+        <v>1</v>
+      </c>
+      <c r="F100" s="17">
+        <v>0</v>
+      </c>
+      <c r="G100" s="17">
+        <v>2</v>
+      </c>
       <c r="H100" s="1">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I100" s="24">
         <v>97</v>
@@ -12760,7 +12855,7 @@
     <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" s="19">
         <f>SUM(H95:H101)</f>
-        <v>14.5</v>
+        <v>26</v>
       </c>
       <c r="B103" s="15"/>
       <c r="C103" s="15"/>

</xml_diff>

<commit_message>
Out of my mind and time
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD5D903-7D8A-4631-8D68-9F7D1F8BD5AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE8656A-59D5-4C78-8152-23C0BF6C748F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1030,7 +1030,7 @@
                   <c:v>148.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>223.5</c:v>
+                  <c:v>225.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>172.5</c:v>
@@ -1568,7 +1568,7 @@
                   <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>9.5</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="99">
                   <c:v>0</c:v>
@@ -2308,7 +2308,7 @@
                   <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>9.5</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="99">
                   <c:v>0</c:v>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>223.5</c:v>
+                  <c:v>225.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5068,7 +5068,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9719,7 +9719,7 @@
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>223.5</v>
+        <v>225.5</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
@@ -9735,7 +9735,7 @@
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>933</v>
+        <v>935</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -12890,7 +12890,7 @@
         <v>1</v>
       </c>
       <c r="D102" s="15">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E102" s="15">
         <v>0.5</v>
@@ -12903,7 +12903,7 @@
       </c>
       <c r="H102" s="1">
         <f t="shared" ref="H102:H107" si="11">SUM(B102:G102)</f>
-        <v>9.5</v>
+        <v>11.5</v>
       </c>
       <c r="I102" s="24">
         <v>99</v>
@@ -13054,7 +13054,7 @@
     <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110" s="14">
         <f>SUM(H102:H108)</f>
-        <v>9.5</v>
+        <v>11.5</v>
       </c>
       <c r="B110" s="17"/>
       <c r="C110" s="17"/>

</xml_diff>

<commit_message>
Doing what I want not what I should
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF7320A-7264-4DE2-9EDF-C8666BF00F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C5DF28-6E52-43E8-8973-B91B40D4FCD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1030,7 +1030,7 @@
                   <c:v>149</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>227</c:v>
+                  <c:v>229.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>175</c:v>
@@ -1039,7 +1039,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>217.5</c:v>
+                  <c:v>218</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1574,7 +1574,7 @@
                   <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>2.5</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="101">
                   <c:v>0</c:v>
@@ -2314,7 +2314,7 @@
                   <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>2.5</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="101">
                   <c:v>0</c:v>
@@ -3344,7 +3344,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>227</c:v>
+                  <c:v>229.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3722,7 +3722,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>217.5</c:v>
+                  <c:v>218</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5086,7 +5086,7 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6196,6 +6196,9 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="99">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="100">
                   <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
@@ -9685,7 +9688,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+      <selection activeCell="G105" sqref="G105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9752,7 +9755,7 @@
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
-        <v>227</v>
+        <v>229.5</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
@@ -9764,11 +9767,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>217.5</v>
+        <v>218</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>950.5</v>
+        <v>953.5</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -12987,7 +12990,7 @@
         <v>0.5</v>
       </c>
       <c r="D104" s="15">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="E104" s="15">
         <v>1</v>
@@ -12995,10 +12998,12 @@
       <c r="F104" s="15">
         <v>0</v>
       </c>
-      <c r="G104" s="15"/>
+      <c r="G104" s="15">
+        <v>0.5</v>
+      </c>
       <c r="H104" s="1">
         <f t="shared" si="11"/>
-        <v>2.5</v>
+        <v>5.5</v>
       </c>
       <c r="I104" s="24">
         <v>101</v>
@@ -13109,7 +13114,7 @@
     <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110" s="14">
         <f>SUM(H102:H108)</f>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B110" s="17"/>
       <c r="C110" s="17"/>

</xml_diff>